<commit_message>
Change output power to -7 dBm. Calculate BER(OSNR)
</commit_message>
<xml_diff>
--- a/APD+FILT+TIA+LIA.xlsx
+++ b/APD+FILT+TIA+LIA.xlsx
@@ -1,18 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10910"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bazarov\Desktop\карантин\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timur/Desktop/карантин/BERvsQfactor/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F2E7918-9C36-1D47-969D-A61CC8D7E22C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="8115"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="14400" windowHeight="8120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name=" Выходная мощность 3 дБм" sheetId="1" r:id="rId1"/>
+    <sheet name="Выходная мощность -7 дБм" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="7">
   <si>
     <t>OSNR, dB</t>
   </si>
@@ -50,7 +52,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -87,7 +89,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -364,21 +366,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y105"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="11" max="11" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="19.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -428,7 +430,7 @@
         <v>4096</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>10</v>
       </c>
@@ -479,7 +481,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>11</v>
       </c>
@@ -529,7 +531,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>12</v>
       </c>
@@ -579,7 +581,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>13</v>
       </c>
@@ -617,7 +619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>14</v>
       </c>
@@ -655,7 +657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>15</v>
       </c>
@@ -693,7 +695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>16</v>
       </c>
@@ -731,7 +733,7 @@
         <v>36.715424749999997</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>17</v>
       </c>
@@ -769,7 +771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>18</v>
       </c>
@@ -807,7 +809,7 @@
         <v>46.142263110000002</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>19</v>
       </c>
@@ -845,7 +847,7 @@
         <v>31.801621059999999</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>20</v>
       </c>
@@ -883,7 +885,7 @@
         <v>35.793208190000001</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>21</v>
       </c>
@@ -912,7 +914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>22</v>
       </c>
@@ -941,7 +943,7 @@
         <v>50.009187879999999</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>23</v>
       </c>
@@ -970,7 +972,7 @@
         <v>44.725644870000004</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>24</v>
       </c>
@@ -999,7 +1001,7 @@
         <v>44.844601689999998</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>25</v>
       </c>
@@ -1028,7 +1030,7 @@
         <v>65.486349169999997</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>26</v>
       </c>
@@ -1057,7 +1059,7 @@
         <v>52.099661500000003</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>27</v>
       </c>
@@ -1086,7 +1088,7 @@
         <v>41.299285519999998</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>28</v>
       </c>
@@ -1115,7 +1117,7 @@
         <v>60.050466139999997</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>29</v>
       </c>
@@ -1144,7 +1146,7 @@
         <v>41.15765931</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>30</v>
       </c>
@@ -1173,7 +1175,7 @@
         <v>55.80791069</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
       <c r="F23" s="2">
         <v>14.05</v>
       </c>
@@ -1184,7 +1186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
       <c r="F24" s="2">
         <v>14.1</v>
       </c>
@@ -1195,7 +1197,7 @@
         <v>21.923804788269052</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
       <c r="F25" s="2">
         <v>14.15</v>
       </c>
@@ -1206,7 +1208,7 @@
         <v>15.818238895820357</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
       <c r="F26" s="2">
         <v>14.2</v>
       </c>
@@ -1217,7 +1219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
       <c r="F27" s="2">
         <v>14.25</v>
       </c>
@@ -1228,7 +1230,7 @@
         <v>22.571762253419433</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
       <c r="F28" s="2">
         <v>14.3</v>
       </c>
@@ -1239,7 +1241,7 @@
         <v>20.146187070620201</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
       <c r="F29" s="2">
         <v>14.35</v>
       </c>
@@ -1250,7 +1252,7 @@
         <v>22.761496379307498</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
       <c r="F30" s="2">
         <v>14.4</v>
       </c>
@@ -1261,7 +1263,7 @@
         <v>18.492257576200338</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
       <c r="F31" s="2">
         <v>14.45</v>
       </c>
@@ -1272,7 +1274,7 @@
         <v>38.018732940327908</v>
       </c>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
       <c r="F32" s="2">
         <v>14.5</v>
       </c>
@@ -1283,7 +1285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F33" s="2">
         <v>14.55</v>
       </c>
@@ -1294,7 +1296,7 @@
         <v>24.202416892605108</v>
       </c>
     </row>
-    <row r="34" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F34" s="2">
         <v>14.6</v>
       </c>
@@ -1305,7 +1307,7 @@
         <v>33.512001361147192</v>
       </c>
     </row>
-    <row r="35" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F35" s="2">
         <v>14.65</v>
       </c>
@@ -1316,7 +1318,7 @@
         <v>19.354848602390042</v>
       </c>
     </row>
-    <row r="36" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F36" s="2">
         <v>14.7</v>
       </c>
@@ -1327,7 +1329,7 @@
         <v>37.870830566345823</v>
       </c>
     </row>
-    <row r="37" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F37" s="2">
         <v>14.75</v>
       </c>
@@ -1338,7 +1340,7 @@
         <v>28.187437108097225</v>
       </c>
     </row>
-    <row r="38" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F38" s="2">
         <v>14.8</v>
       </c>
@@ -1349,7 +1351,7 @@
         <v>35.916238682920643</v>
       </c>
     </row>
-    <row r="39" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F39" s="2">
         <v>14.85</v>
       </c>
@@ -1360,7 +1362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F40" s="2">
         <v>14.9</v>
       </c>
@@ -1371,7 +1373,7 @@
         <v>31.113041251633398</v>
       </c>
     </row>
-    <row r="41" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F41" s="2">
         <v>14.95</v>
       </c>
@@ -1382,7 +1384,7 @@
         <v>23.624746072673169</v>
       </c>
     </row>
-    <row r="42" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F42" s="2">
         <v>15</v>
       </c>
@@ -1393,7 +1395,7 @@
         <v>41.177848027343934</v>
       </c>
     </row>
-    <row r="43" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F43">
         <v>15</v>
       </c>
@@ -1404,7 +1406,7 @@
         <v>49.888300299999997</v>
       </c>
     </row>
-    <row r="44" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F44">
         <v>15.05</v>
       </c>
@@ -1415,7 +1417,7 @@
         <v>32.567680510000002</v>
       </c>
     </row>
-    <row r="45" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F45">
         <v>15.1</v>
       </c>
@@ -1426,7 +1428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F46">
         <v>15.15</v>
       </c>
@@ -1437,7 +1439,7 @@
         <v>31.7298334</v>
       </c>
     </row>
-    <row r="47" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F47">
         <v>15.2</v>
       </c>
@@ -1448,7 +1450,7 @@
         <v>20.002188159999999</v>
       </c>
     </row>
-    <row r="48" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F48">
         <v>15.25</v>
       </c>
@@ -1459,7 +1461,7 @@
         <v>49.216737330000001</v>
       </c>
     </row>
-    <row r="49" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F49">
         <v>15.3</v>
       </c>
@@ -1470,7 +1472,7 @@
         <v>40.500207029999999</v>
       </c>
     </row>
-    <row r="50" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F50">
         <v>15.35</v>
       </c>
@@ -1481,7 +1483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F51">
         <v>15.4</v>
       </c>
@@ -1492,7 +1494,7 @@
         <v>50.94129813</v>
       </c>
     </row>
-    <row r="52" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F52">
         <v>15.45</v>
       </c>
@@ -1503,7 +1505,7 @@
         <v>34.551906680000002</v>
       </c>
     </row>
-    <row r="53" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F53">
         <v>15.5</v>
       </c>
@@ -1514,7 +1516,7 @@
         <v>33.957837589999997</v>
       </c>
     </row>
-    <row r="54" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F54">
         <v>15.55</v>
       </c>
@@ -1525,7 +1527,7 @@
         <v>34.939419149999999</v>
       </c>
     </row>
-    <row r="55" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F55">
         <v>15.6</v>
       </c>
@@ -1536,7 +1538,7 @@
         <v>20.697958239999998</v>
       </c>
     </row>
-    <row r="56" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F56">
         <v>15.65</v>
       </c>
@@ -1547,7 +1549,7 @@
         <v>39.345351139999998</v>
       </c>
     </row>
-    <row r="57" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F57">
         <v>15.7</v>
       </c>
@@ -1558,7 +1560,7 @@
         <v>50.907188470000001</v>
       </c>
     </row>
-    <row r="58" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F58">
         <v>15.75</v>
       </c>
@@ -1569,7 +1571,7 @@
         <v>47.395161469999998</v>
       </c>
     </row>
-    <row r="59" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F59">
         <v>15.8</v>
       </c>
@@ -1580,7 +1582,7 @@
         <v>58.185976289999999</v>
       </c>
     </row>
-    <row r="60" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F60">
         <v>15.85</v>
       </c>
@@ -1591,7 +1593,7 @@
         <v>53.899870579999998</v>
       </c>
     </row>
-    <row r="61" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F61">
         <v>15.9</v>
       </c>
@@ -1602,7 +1604,7 @@
         <v>19.606000890000001</v>
       </c>
     </row>
-    <row r="62" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F62">
         <v>15.95</v>
       </c>
@@ -1613,7 +1615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F63">
         <v>16</v>
       </c>
@@ -1624,7 +1626,7 @@
         <v>58.331122120000003</v>
       </c>
     </row>
-    <row r="64" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F64">
         <v>16</v>
       </c>
@@ -1635,7 +1637,7 @@
         <v>44.640776430000003</v>
       </c>
     </row>
-    <row r="65" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F65">
         <v>16.05</v>
       </c>
@@ -1646,7 +1648,7 @@
         <v>39.888597079999997</v>
       </c>
     </row>
-    <row r="66" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F66">
         <v>16.100000000000001</v>
       </c>
@@ -1657,7 +1659,7 @@
         <v>26.38694267</v>
       </c>
     </row>
-    <row r="67" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F67">
         <v>16.149999999999999</v>
       </c>
@@ -1668,7 +1670,7 @@
         <v>56.199351980000003</v>
       </c>
     </row>
-    <row r="68" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F68">
         <v>16.2</v>
       </c>
@@ -1679,7 +1681,7 @@
         <v>63.583161869999998</v>
       </c>
     </row>
-    <row r="69" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F69">
         <v>16.25</v>
       </c>
@@ -1690,7 +1692,7 @@
         <v>47.76873174</v>
       </c>
     </row>
-    <row r="70" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F70">
         <v>16.3</v>
       </c>
@@ -1701,7 +1703,7 @@
         <v>36.604562540000003</v>
       </c>
     </row>
-    <row r="71" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F71">
         <v>16.350000000000001</v>
       </c>
@@ -1712,7 +1714,7 @@
         <v>47.181701400000001</v>
       </c>
     </row>
-    <row r="72" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F72">
         <v>16.399999999999999</v>
       </c>
@@ -1723,7 +1725,7 @@
         <v>45.44361576</v>
       </c>
     </row>
-    <row r="73" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F73">
         <v>16.45</v>
       </c>
@@ -1734,7 +1736,7 @@
         <v>64.086472720000003</v>
       </c>
     </row>
-    <row r="74" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F74">
         <v>16.5</v>
       </c>
@@ -1745,7 +1747,7 @@
         <v>47.398998470000002</v>
       </c>
     </row>
-    <row r="75" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F75">
         <v>16.55</v>
       </c>
@@ -1756,7 +1758,7 @@
         <v>68.418190089999996</v>
       </c>
     </row>
-    <row r="76" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F76">
         <v>16.600000000000001</v>
       </c>
@@ -1767,7 +1769,7 @@
         <v>55.158037200000003</v>
       </c>
     </row>
-    <row r="77" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F77">
         <v>16.649999999999999</v>
       </c>
@@ -1778,7 +1780,7 @@
         <v>50.885233759999998</v>
       </c>
     </row>
-    <row r="78" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F78">
         <v>16.7</v>
       </c>
@@ -1789,7 +1791,7 @@
         <v>60.989703810000002</v>
       </c>
     </row>
-    <row r="79" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F79">
         <v>16.75</v>
       </c>
@@ -1800,7 +1802,7 @@
         <v>51.063679800000003</v>
       </c>
     </row>
-    <row r="80" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F80">
         <v>16.8</v>
       </c>
@@ -1811,7 +1813,7 @@
         <v>61.377824429999997</v>
       </c>
     </row>
-    <row r="81" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F81">
         <v>16.850000000000001</v>
       </c>
@@ -1822,7 +1824,7 @@
         <v>50.586775950000003</v>
       </c>
     </row>
-    <row r="82" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F82">
         <v>16.899999999999999</v>
       </c>
@@ -1833,7 +1835,7 @@
         <v>58.532791699999997</v>
       </c>
     </row>
-    <row r="83" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F83">
         <v>16.95</v>
       </c>
@@ -1844,7 +1846,7 @@
         <v>74.290789899999993</v>
       </c>
     </row>
-    <row r="84" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F84">
         <v>17</v>
       </c>
@@ -1855,7 +1857,7 @@
         <v>53.737096049999998</v>
       </c>
     </row>
-    <row r="85" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F85">
         <v>17</v>
       </c>
@@ -1866,7 +1868,7 @@
         <v>64.608913099999995</v>
       </c>
     </row>
-    <row r="86" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F86">
         <v>17.05</v>
       </c>
@@ -1877,7 +1879,7 @@
         <v>55.91</v>
       </c>
     </row>
-    <row r="87" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F87">
         <v>17.100000000000001</v>
       </c>
@@ -1888,7 +1890,7 @@
         <v>59.215105489999999</v>
       </c>
     </row>
-    <row r="88" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F88">
         <v>17.149999999999999</v>
       </c>
@@ -1899,7 +1901,7 @@
         <v>60.950603540000003</v>
       </c>
     </row>
-    <row r="89" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F89">
         <v>17.2</v>
       </c>
@@ -1910,7 +1912,7 @@
         <v>65.05784036</v>
       </c>
     </row>
-    <row r="90" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F90">
         <v>17.25</v>
       </c>
@@ -1921,7 +1923,7 @@
         <v>61.199202550000003</v>
       </c>
     </row>
-    <row r="91" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F91">
         <v>17.3</v>
       </c>
@@ -1932,7 +1934,7 @@
         <v>69.028638139999998</v>
       </c>
     </row>
-    <row r="92" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F92">
         <v>17.350000000000001</v>
       </c>
@@ -1943,7 +1945,7 @@
         <v>66.15736004</v>
       </c>
     </row>
-    <row r="93" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F93">
         <v>17.399999999999999</v>
       </c>
@@ -1954,7 +1956,7 @@
         <v>67.575601829999997</v>
       </c>
     </row>
-    <row r="94" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F94">
         <v>17.45</v>
       </c>
@@ -1965,7 +1967,7 @@
         <v>62.257543239999997</v>
       </c>
     </row>
-    <row r="95" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F95">
         <v>17.5</v>
       </c>
@@ -1976,7 +1978,7 @@
         <v>67.212681610000004</v>
       </c>
     </row>
-    <row r="96" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F96">
         <v>17.55</v>
       </c>
@@ -1987,7 +1989,7 @@
         <v>65.830806339999995</v>
       </c>
     </row>
-    <row r="97" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F97">
         <v>17.600000000000001</v>
       </c>
@@ -1998,7 +2000,7 @@
         <v>66.418148720000005</v>
       </c>
     </row>
-    <row r="98" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F98">
         <v>17.649999999999999</v>
       </c>
@@ -2009,7 +2011,7 @@
         <v>67.684434940000003</v>
       </c>
     </row>
-    <row r="99" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F99">
         <v>17.7</v>
       </c>
@@ -2020,7 +2022,7 @@
         <v>73.788069730000004</v>
       </c>
     </row>
-    <row r="100" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F100">
         <v>17.75</v>
       </c>
@@ -2031,7 +2033,7 @@
         <v>72.895772750000006</v>
       </c>
     </row>
-    <row r="101" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F101">
         <v>17.8</v>
       </c>
@@ -2042,7 +2044,7 @@
         <v>71.154751680000004</v>
       </c>
     </row>
-    <row r="102" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F102">
         <v>17.850000000000001</v>
       </c>
@@ -2053,7 +2055,7 @@
         <v>68.843598439999994</v>
       </c>
     </row>
-    <row r="103" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F103">
         <v>17.899999999999999</v>
       </c>
@@ -2064,7 +2066,7 @@
         <v>70.726856819999995</v>
       </c>
     </row>
-    <row r="104" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F104">
         <v>17.95</v>
       </c>
@@ -2075,7 +2077,7 @@
         <v>73.816151189999999</v>
       </c>
     </row>
-    <row r="105" spans="6:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F105">
         <v>18</v>
       </c>
@@ -2084,6 +2086,1365 @@
       </c>
       <c r="H105">
         <v>70.327556090000002</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B3CADCF-C2E9-764E-ADBA-D979EDBEAE38}">
+  <dimension ref="A1:L102"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>13</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="K2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>13.05</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="K3" t="s">
+        <v>3</v>
+      </c>
+      <c r="L3">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>13.1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="K4" t="s">
+        <v>4</v>
+      </c>
+      <c r="L4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>13.15</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>14</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>13.2</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>13.25</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>16</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>40.749428279999997</v>
+      </c>
+      <c r="F8">
+        <v>13.3</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>17</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>42.992130230000001</v>
+      </c>
+      <c r="F9">
+        <v>13.35</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>18</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>64.528584080000002</v>
+      </c>
+      <c r="F10">
+        <v>13.4</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>19</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>67.486249790000002</v>
+      </c>
+      <c r="F11">
+        <v>13.45</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>20</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>74.139306219999995</v>
+      </c>
+      <c r="F12">
+        <v>13.5</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>21</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>76.272300779999995</v>
+      </c>
+      <c r="F13">
+        <v>13.55</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>22</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>77.92226651</v>
+      </c>
+      <c r="F14">
+        <v>13.6</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>23</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>79.116974080000006</v>
+      </c>
+      <c r="F15">
+        <v>13.65</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>24</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>79.383310629999997</v>
+      </c>
+      <c r="F16">
+        <v>13.7</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>25</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>79.434057499999994</v>
+      </c>
+      <c r="F17">
+        <v>13.75</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>26</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>79.570946320000004</v>
+      </c>
+      <c r="F18">
+        <v>13.8</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>27</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>80.116235340000003</v>
+      </c>
+      <c r="F19">
+        <v>13.85</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>28</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>79.845306550000004</v>
+      </c>
+      <c r="F20">
+        <v>13.9</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>29</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>80.321418269999995</v>
+      </c>
+      <c r="F21">
+        <v>13.95</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>30</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>79.672660469999997</v>
+      </c>
+      <c r="F22">
+        <v>14</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F23">
+        <v>14.05</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F24">
+        <v>14.1</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F25">
+        <v>14.15</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F26">
+        <v>14.2</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F27">
+        <v>14.25</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F28">
+        <v>14.3</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F29">
+        <v>14.35</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F30">
+        <v>14.4</v>
+      </c>
+      <c r="G30">
+        <v>1</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F31">
+        <v>14.45</v>
+      </c>
+      <c r="G31" s="1">
+        <v>1.11E-100</v>
+      </c>
+      <c r="H31">
+        <v>21.265233550000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F32">
+        <v>14.5</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F33">
+        <v>14.55</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F34">
+        <v>14.6</v>
+      </c>
+      <c r="G34">
+        <v>1</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F35">
+        <v>14.65</v>
+      </c>
+      <c r="G35">
+        <v>1</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F36">
+        <v>14.7</v>
+      </c>
+      <c r="G36" s="1">
+        <v>1.8799999999999998E-108</v>
+      </c>
+      <c r="H36">
+        <v>22.087569550000001</v>
+      </c>
+    </row>
+    <row r="37" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F37">
+        <v>14.75</v>
+      </c>
+      <c r="G37" s="1">
+        <v>1.7599999999999999E-108</v>
+      </c>
+      <c r="H37">
+        <v>22.085593889999998</v>
+      </c>
+    </row>
+    <row r="38" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F38">
+        <v>14.8</v>
+      </c>
+      <c r="G38">
+        <v>1</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F39">
+        <v>14.85</v>
+      </c>
+      <c r="G39">
+        <v>1</v>
+      </c>
+      <c r="H39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F40">
+        <v>14.9</v>
+      </c>
+      <c r="G40" s="1">
+        <v>6.2199999999999999E-206</v>
+      </c>
+      <c r="H40">
+        <v>30.592749470000001</v>
+      </c>
+    </row>
+    <row r="41" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F41">
+        <v>14.95</v>
+      </c>
+      <c r="G41">
+        <v>1</v>
+      </c>
+      <c r="H41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F42">
+        <v>15</v>
+      </c>
+      <c r="G42">
+        <v>1</v>
+      </c>
+      <c r="H42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F43">
+        <v>15.05</v>
+      </c>
+      <c r="G43">
+        <v>1</v>
+      </c>
+      <c r="H43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F44">
+        <v>15.1</v>
+      </c>
+      <c r="G44">
+        <v>1</v>
+      </c>
+      <c r="H44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F45">
+        <v>15.15</v>
+      </c>
+      <c r="G45">
+        <v>0</v>
+      </c>
+      <c r="H45">
+        <v>39.316776590000003</v>
+      </c>
+    </row>
+    <row r="46" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F46">
+        <v>15.2</v>
+      </c>
+      <c r="G46" s="1">
+        <v>2.9700000000000001E-43</v>
+      </c>
+      <c r="H46">
+        <v>13.72634712</v>
+      </c>
+    </row>
+    <row r="47" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F47">
+        <v>15.25</v>
+      </c>
+      <c r="G47">
+        <v>1</v>
+      </c>
+      <c r="H47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F48">
+        <v>15.3</v>
+      </c>
+      <c r="G48">
+        <v>1</v>
+      </c>
+      <c r="H48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F49">
+        <v>15.35</v>
+      </c>
+      <c r="G49" s="1">
+        <v>1.53E-164</v>
+      </c>
+      <c r="H49">
+        <v>27.310688150000001</v>
+      </c>
+    </row>
+    <row r="50" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F50">
+        <v>15.4</v>
+      </c>
+      <c r="G50" s="1">
+        <v>3.4400000000000001E-154</v>
+      </c>
+      <c r="H50">
+        <v>26.42082826</v>
+      </c>
+    </row>
+    <row r="51" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F51">
+        <v>15.45</v>
+      </c>
+      <c r="G51">
+        <v>0</v>
+      </c>
+      <c r="H51">
+        <v>40.48602588</v>
+      </c>
+    </row>
+    <row r="52" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F52">
+        <v>15.5</v>
+      </c>
+      <c r="G52">
+        <v>1</v>
+      </c>
+      <c r="H52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F53">
+        <v>15.55</v>
+      </c>
+      <c r="G53">
+        <v>0</v>
+      </c>
+      <c r="H53">
+        <v>38.85373053</v>
+      </c>
+    </row>
+    <row r="54" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F54">
+        <v>15.6</v>
+      </c>
+      <c r="G54">
+        <v>1</v>
+      </c>
+      <c r="H54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F55">
+        <v>15.65</v>
+      </c>
+      <c r="G55" s="1">
+        <v>5.6299999999999998E-236</v>
+      </c>
+      <c r="H55">
+        <v>32.774403270000001</v>
+      </c>
+    </row>
+    <row r="56" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F56">
+        <v>15.7</v>
+      </c>
+      <c r="G56" s="1">
+        <v>1.03E-209</v>
+      </c>
+      <c r="H56">
+        <v>30.87977849</v>
+      </c>
+    </row>
+    <row r="57" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F57">
+        <v>15.75</v>
+      </c>
+      <c r="G57" s="1">
+        <v>1.27E-256</v>
+      </c>
+      <c r="H57">
+        <v>34.197245649999999</v>
+      </c>
+    </row>
+    <row r="58" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F58">
+        <v>15.8</v>
+      </c>
+      <c r="G58">
+        <v>1</v>
+      </c>
+      <c r="H58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F59">
+        <v>15.85</v>
+      </c>
+      <c r="G59">
+        <v>0</v>
+      </c>
+      <c r="H59">
+        <v>40.687379040000003</v>
+      </c>
+    </row>
+    <row r="60" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F60">
+        <v>15.9</v>
+      </c>
+      <c r="G60">
+        <v>1</v>
+      </c>
+      <c r="H60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F61">
+        <v>15.95</v>
+      </c>
+      <c r="G61">
+        <v>0</v>
+      </c>
+      <c r="H61">
+        <v>50.276012389999998</v>
+      </c>
+    </row>
+    <row r="62" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F62">
+        <v>16</v>
+      </c>
+      <c r="G62">
+        <v>0</v>
+      </c>
+      <c r="H62">
+        <v>40.184062750000002</v>
+      </c>
+    </row>
+    <row r="63" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F63">
+        <v>16.05</v>
+      </c>
+      <c r="G63" s="1">
+        <v>1.17E-292</v>
+      </c>
+      <c r="H63">
+        <v>36.540523759999999</v>
+      </c>
+    </row>
+    <row r="64" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F64">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="G64" s="1">
+        <v>5.2499999999999996E-230</v>
+      </c>
+      <c r="H64">
+        <v>32.358304269999998</v>
+      </c>
+    </row>
+    <row r="65" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F65">
+        <v>16.149999999999999</v>
+      </c>
+      <c r="G65">
+        <v>0</v>
+      </c>
+      <c r="H65">
+        <v>46.143615660000002</v>
+      </c>
+    </row>
+    <row r="66" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F66">
+        <v>16.2</v>
+      </c>
+      <c r="G66">
+        <v>0</v>
+      </c>
+      <c r="H66">
+        <v>48.784062069999997</v>
+      </c>
+    </row>
+    <row r="67" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F67">
+        <v>16.25</v>
+      </c>
+      <c r="G67">
+        <v>0</v>
+      </c>
+      <c r="H67">
+        <v>48.321877540000003</v>
+      </c>
+    </row>
+    <row r="68" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F68">
+        <v>16.3</v>
+      </c>
+      <c r="G68">
+        <v>0</v>
+      </c>
+      <c r="H68">
+        <v>49.631022489999999</v>
+      </c>
+    </row>
+    <row r="69" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F69">
+        <v>16.350000000000001</v>
+      </c>
+      <c r="G69">
+        <v>0</v>
+      </c>
+      <c r="H69">
+        <v>49.468441429999999</v>
+      </c>
+    </row>
+    <row r="70" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F70">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="G70">
+        <v>0</v>
+      </c>
+      <c r="H70">
+        <v>52.660545939999999</v>
+      </c>
+    </row>
+    <row r="71" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F71">
+        <v>16.45</v>
+      </c>
+      <c r="G71">
+        <v>0</v>
+      </c>
+      <c r="H71">
+        <v>48.46359064</v>
+      </c>
+    </row>
+    <row r="72" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F72">
+        <v>16.5</v>
+      </c>
+      <c r="G72">
+        <v>0</v>
+      </c>
+      <c r="H72">
+        <v>50.266107259999998</v>
+      </c>
+    </row>
+    <row r="73" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F73">
+        <v>16.55</v>
+      </c>
+      <c r="G73">
+        <v>0</v>
+      </c>
+      <c r="H73">
+        <v>49.301880369999999</v>
+      </c>
+    </row>
+    <row r="74" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F74">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="G74">
+        <v>0</v>
+      </c>
+      <c r="H74">
+        <v>54.586823500000001</v>
+      </c>
+    </row>
+    <row r="75" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F75">
+        <v>16.649999999999999</v>
+      </c>
+      <c r="G75">
+        <v>0</v>
+      </c>
+      <c r="H75">
+        <v>56.198574569999998</v>
+      </c>
+    </row>
+    <row r="76" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F76">
+        <v>16.7</v>
+      </c>
+      <c r="G76">
+        <v>0</v>
+      </c>
+      <c r="H76">
+        <v>48.004052420000001</v>
+      </c>
+    </row>
+    <row r="77" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F77">
+        <v>16.75</v>
+      </c>
+      <c r="G77">
+        <v>0</v>
+      </c>
+      <c r="H77">
+        <v>57.658728979999999</v>
+      </c>
+    </row>
+    <row r="78" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F78">
+        <v>16.8</v>
+      </c>
+      <c r="G78">
+        <v>0</v>
+      </c>
+      <c r="H78">
+        <v>55.133515600000003</v>
+      </c>
+    </row>
+    <row r="79" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F79">
+        <v>16.850000000000001</v>
+      </c>
+      <c r="G79">
+        <v>0</v>
+      </c>
+      <c r="H79">
+        <v>54.759498260000001</v>
+      </c>
+    </row>
+    <row r="80" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F80">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="G80">
+        <v>0</v>
+      </c>
+      <c r="H80">
+        <v>56.173744980000002</v>
+      </c>
+    </row>
+    <row r="81" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F81">
+        <v>16.95</v>
+      </c>
+      <c r="G81">
+        <v>0</v>
+      </c>
+      <c r="H81">
+        <v>61.166705929999999</v>
+      </c>
+    </row>
+    <row r="82" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F82">
+        <v>17</v>
+      </c>
+      <c r="G82">
+        <v>0</v>
+      </c>
+      <c r="H82">
+        <v>58.002330290000003</v>
+      </c>
+    </row>
+    <row r="83" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F83">
+        <v>17.05</v>
+      </c>
+      <c r="G83">
+        <v>0</v>
+      </c>
+      <c r="H83">
+        <v>51.670730460000001</v>
+      </c>
+    </row>
+    <row r="84" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F84">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="G84">
+        <v>0</v>
+      </c>
+      <c r="H84">
+        <v>53.79423895</v>
+      </c>
+    </row>
+    <row r="85" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F85">
+        <v>17.149999999999999</v>
+      </c>
+      <c r="G85">
+        <v>0</v>
+      </c>
+      <c r="H85">
+        <v>62.20640968</v>
+      </c>
+    </row>
+    <row r="86" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F86">
+        <v>17.2</v>
+      </c>
+      <c r="G86">
+        <v>0</v>
+      </c>
+      <c r="H86">
+        <v>62.61363283</v>
+      </c>
+    </row>
+    <row r="87" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F87">
+        <v>17.25</v>
+      </c>
+      <c r="G87">
+        <v>0</v>
+      </c>
+      <c r="H87">
+        <v>63.690048509999997</v>
+      </c>
+    </row>
+    <row r="88" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F88">
+        <v>17.3</v>
+      </c>
+      <c r="G88">
+        <v>0</v>
+      </c>
+      <c r="H88">
+        <v>47.30045527</v>
+      </c>
+    </row>
+    <row r="89" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F89">
+        <v>17.350000000000001</v>
+      </c>
+      <c r="G89">
+        <v>0</v>
+      </c>
+      <c r="H89">
+        <v>58.132979720000002</v>
+      </c>
+    </row>
+    <row r="90" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F90">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="G90">
+        <v>0</v>
+      </c>
+      <c r="H90">
+        <v>57.941216750000002</v>
+      </c>
+    </row>
+    <row r="91" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F91">
+        <v>17.45</v>
+      </c>
+      <c r="G91">
+        <v>0</v>
+      </c>
+      <c r="H91">
+        <v>58.118236099999997</v>
+      </c>
+    </row>
+    <row r="92" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F92">
+        <v>17.5</v>
+      </c>
+      <c r="G92">
+        <v>0</v>
+      </c>
+      <c r="H92">
+        <v>56.37006178</v>
+      </c>
+    </row>
+    <row r="93" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F93">
+        <v>17.55</v>
+      </c>
+      <c r="G93">
+        <v>0</v>
+      </c>
+      <c r="H93">
+        <v>65.745433449999993</v>
+      </c>
+    </row>
+    <row r="94" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F94">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="G94">
+        <v>0</v>
+      </c>
+      <c r="H94">
+        <v>64.373812709999996</v>
+      </c>
+    </row>
+    <row r="95" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F95">
+        <v>17.649999999999999</v>
+      </c>
+      <c r="G95">
+        <v>0</v>
+      </c>
+      <c r="H95">
+        <v>63.078113960000003</v>
+      </c>
+    </row>
+    <row r="96" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F96">
+        <v>17.7</v>
+      </c>
+      <c r="G96">
+        <v>0</v>
+      </c>
+      <c r="H96">
+        <v>63.403778580000001</v>
+      </c>
+    </row>
+    <row r="97" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F97">
+        <v>17.75</v>
+      </c>
+      <c r="G97">
+        <v>0</v>
+      </c>
+      <c r="H97">
+        <v>69.787713010000004</v>
+      </c>
+    </row>
+    <row r="98" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F98">
+        <v>17.8</v>
+      </c>
+      <c r="G98">
+        <v>0</v>
+      </c>
+      <c r="H98">
+        <v>59.474370010000001</v>
+      </c>
+    </row>
+    <row r="99" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F99">
+        <v>17.850000000000001</v>
+      </c>
+      <c r="G99">
+        <v>0</v>
+      </c>
+      <c r="H99">
+        <v>57.372991579999997</v>
+      </c>
+    </row>
+    <row r="100" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F100">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="G100">
+        <v>0</v>
+      </c>
+      <c r="H100">
+        <v>67.558118289999996</v>
+      </c>
+    </row>
+    <row r="101" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F101">
+        <v>17.95</v>
+      </c>
+      <c r="G101">
+        <v>0</v>
+      </c>
+      <c r="H101">
+        <v>65.243549740000006</v>
+      </c>
+    </row>
+    <row r="102" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F102">
+        <v>18</v>
+      </c>
+      <c r="G102">
+        <v>0</v>
+      </c>
+      <c r="H102">
+        <v>64.305960569999996</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Gain of output amplifier is 0
</commit_message>
<xml_diff>
--- a/APD+FILT+TIA+LIA.xlsx
+++ b/APD+FILT+TIA+LIA.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timur/Desktop/карантин/BERvsQfactor/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F2E7918-9C36-1D47-969D-A61CC8D7E22C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF02A6E7-24D4-AB40-8CD2-AE1726229D34}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="14400" windowHeight="8120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="14400" windowHeight="8120" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name=" Выходная мощность 3 дБм" sheetId="1" r:id="rId1"/>
     <sheet name="Выходная мощность -7 дБм" sheetId="2" r:id="rId2"/>
+    <sheet name="Gain of output ampl = 0" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="7">
   <si>
     <t>OSNR, dB</t>
   </si>
@@ -2097,7 +2098,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B3CADCF-C2E9-764E-ADBA-D979EDBEAE38}">
   <dimension ref="A1:L102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -3450,4 +3451,1363 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D12F1B7-876E-D145-8035-611196C117A8}">
+  <dimension ref="A1:L102"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:L102"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>13</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="K2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>13.05</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1.24E-36</v>
+      </c>
+      <c r="H3">
+        <v>12.57009278</v>
+      </c>
+      <c r="K3" t="s">
+        <v>3</v>
+      </c>
+      <c r="L3">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>13.1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="K4" t="s">
+        <v>4</v>
+      </c>
+      <c r="L4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>13.15</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>14</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>13.2</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>15</v>
+      </c>
+      <c r="B7" s="1">
+        <v>8.8899999999999996E-135</v>
+      </c>
+      <c r="C7">
+        <v>24.678745360000001</v>
+      </c>
+      <c r="F7">
+        <v>13.25</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>16</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1.91E-208</v>
+      </c>
+      <c r="C8">
+        <v>30.78020399</v>
+      </c>
+      <c r="F8">
+        <v>13.3</v>
+      </c>
+      <c r="G8" s="1">
+        <v>5.3399999999999998E-40</v>
+      </c>
+      <c r="H8">
+        <v>13.178291440000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>17</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>47.975084449999997</v>
+      </c>
+      <c r="F9">
+        <v>13.35</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>18</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>74.096946169999995</v>
+      </c>
+      <c r="F10">
+        <v>13.4</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>19</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>71.2774912</v>
+      </c>
+      <c r="F11">
+        <v>13.45</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>20</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>67.124044290000001</v>
+      </c>
+      <c r="F12">
+        <v>13.5</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>21</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>77.086549349999999</v>
+      </c>
+      <c r="F13">
+        <v>13.55</v>
+      </c>
+      <c r="G13" s="1">
+        <v>9.0199999999999995E-37</v>
+      </c>
+      <c r="H13">
+        <v>12.599213239999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>22</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>78.646314410000002</v>
+      </c>
+      <c r="F14">
+        <v>13.6</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>23</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>78.640877590000002</v>
+      </c>
+      <c r="F15">
+        <v>13.65</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>24</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>80.419444839999997</v>
+      </c>
+      <c r="F16">
+        <v>13.7</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>25</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>80.796233369999996</v>
+      </c>
+      <c r="F17">
+        <v>13.75</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>26</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>80.633016049999995</v>
+      </c>
+      <c r="F18">
+        <v>13.8</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>27</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>81.272811559999994</v>
+      </c>
+      <c r="F19">
+        <v>13.85</v>
+      </c>
+      <c r="G19" s="1">
+        <v>4.0799999999999999E-77</v>
+      </c>
+      <c r="H19">
+        <v>18.544439000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>28</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>80.538175469999999</v>
+      </c>
+      <c r="F20">
+        <v>13.9</v>
+      </c>
+      <c r="G20" s="1">
+        <v>1.69E-59</v>
+      </c>
+      <c r="H20">
+        <v>16.220817419999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>29</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>81.335496739999996</v>
+      </c>
+      <c r="F21">
+        <v>13.95</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>30</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>81.455940389999995</v>
+      </c>
+      <c r="F22">
+        <v>14</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F23">
+        <v>14.05</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F24">
+        <v>14.1</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F25">
+        <v>14.15</v>
+      </c>
+      <c r="G25" s="1">
+        <v>1.72E-77</v>
+      </c>
+      <c r="H25">
+        <v>18.594508260000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F26">
+        <v>14.2</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F27">
+        <v>14.25</v>
+      </c>
+      <c r="G27" s="1">
+        <v>9.0499999999999997E-55</v>
+      </c>
+      <c r="H27">
+        <v>15.53918593</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F28">
+        <v>14.3</v>
+      </c>
+      <c r="G28" s="1">
+        <v>2.1599999999999999E-131</v>
+      </c>
+      <c r="H28">
+        <v>24.34941796</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F29">
+        <v>14.35</v>
+      </c>
+      <c r="G29" s="1">
+        <v>2.35E-84</v>
+      </c>
+      <c r="H29">
+        <v>19.413732889999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F30">
+        <v>14.4</v>
+      </c>
+      <c r="G30" s="1">
+        <v>1.04E-54</v>
+      </c>
+      <c r="H30">
+        <v>15.512140069999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F31">
+        <v>14.45</v>
+      </c>
+      <c r="G31" s="1">
+        <v>5.4000000000000003E-82</v>
+      </c>
+      <c r="H31">
+        <v>19.14423648</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F32">
+        <v>14.5</v>
+      </c>
+      <c r="G32" s="1">
+        <v>1.1100000000000001E-56</v>
+      </c>
+      <c r="H32">
+        <v>15.809940920000001</v>
+      </c>
+    </row>
+    <row r="33" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F33">
+        <v>14.55</v>
+      </c>
+      <c r="G33" s="1">
+        <v>7.9000000000000003E-40</v>
+      </c>
+      <c r="H33">
+        <v>13.153591540000001</v>
+      </c>
+    </row>
+    <row r="34" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F34">
+        <v>14.6</v>
+      </c>
+      <c r="G34" s="1">
+        <v>2.6700000000000001E-70</v>
+      </c>
+      <c r="H34">
+        <v>17.684677220000001</v>
+      </c>
+    </row>
+    <row r="35" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F35">
+        <v>14.65</v>
+      </c>
+      <c r="G35" s="1">
+        <v>4.5700000000000003E-68</v>
+      </c>
+      <c r="H35">
+        <v>17.390476799999998</v>
+      </c>
+    </row>
+    <row r="36" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F36">
+        <v>14.7</v>
+      </c>
+      <c r="G36">
+        <v>1</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F37">
+        <v>14.75</v>
+      </c>
+      <c r="G37" s="1">
+        <v>2.0499999999999999E-70</v>
+      </c>
+      <c r="H37">
+        <v>17.6994434</v>
+      </c>
+    </row>
+    <row r="38" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F38">
+        <v>14.8</v>
+      </c>
+      <c r="G38">
+        <v>1</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F39">
+        <v>14.85</v>
+      </c>
+      <c r="G39" s="1">
+        <v>1.92E-66</v>
+      </c>
+      <c r="H39">
+        <v>17.15513992</v>
+      </c>
+    </row>
+    <row r="40" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F40">
+        <v>14.9</v>
+      </c>
+      <c r="G40" s="1">
+        <v>5.28E-140</v>
+      </c>
+      <c r="H40">
+        <v>25.157585560000001</v>
+      </c>
+    </row>
+    <row r="41" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F41">
+        <v>14.95</v>
+      </c>
+      <c r="G41" s="1">
+        <v>1.04E-132</v>
+      </c>
+      <c r="H41">
+        <v>24.486042560000001</v>
+      </c>
+    </row>
+    <row r="42" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F42">
+        <v>15</v>
+      </c>
+      <c r="G42" s="1">
+        <v>1.43E-133</v>
+      </c>
+      <c r="H42">
+        <v>24.561293599999999</v>
+      </c>
+    </row>
+    <row r="43" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F43">
+        <v>15.05</v>
+      </c>
+      <c r="G43" s="1">
+        <v>5.5100000000000003E-282</v>
+      </c>
+      <c r="H43">
+        <v>35.862747110000001</v>
+      </c>
+    </row>
+    <row r="44" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F44">
+        <v>15.1</v>
+      </c>
+      <c r="G44" s="1">
+        <v>2.41E-85</v>
+      </c>
+      <c r="H44">
+        <v>19.526974160000002</v>
+      </c>
+    </row>
+    <row r="45" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F45">
+        <v>15.15</v>
+      </c>
+      <c r="G45" s="1">
+        <v>1.5400000000000001E-50</v>
+      </c>
+      <c r="H45">
+        <v>14.90341096</v>
+      </c>
+    </row>
+    <row r="46" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F46">
+        <v>15.2</v>
+      </c>
+      <c r="G46">
+        <v>0</v>
+      </c>
+      <c r="H46">
+        <v>41.07759995</v>
+      </c>
+    </row>
+    <row r="47" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F47">
+        <v>15.25</v>
+      </c>
+      <c r="G47" s="1">
+        <v>4.3400000000000004E-205</v>
+      </c>
+      <c r="H47">
+        <v>30.528617000000001</v>
+      </c>
+    </row>
+    <row r="48" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F48">
+        <v>15.3</v>
+      </c>
+      <c r="G48" s="1">
+        <v>2.6E-220</v>
+      </c>
+      <c r="H48">
+        <v>31.661665230000001</v>
+      </c>
+    </row>
+    <row r="49" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F49">
+        <v>15.35</v>
+      </c>
+      <c r="G49" s="1">
+        <v>5.7499999999999997E-174</v>
+      </c>
+      <c r="H49">
+        <v>28.085272920000001</v>
+      </c>
+    </row>
+    <row r="50" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F50">
+        <v>15.4</v>
+      </c>
+      <c r="G50" s="1">
+        <v>1.58E-83</v>
+      </c>
+      <c r="H50">
+        <v>19.309263569999999</v>
+      </c>
+    </row>
+    <row r="51" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F51">
+        <v>15.45</v>
+      </c>
+      <c r="G51">
+        <v>1</v>
+      </c>
+      <c r="H51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F52">
+        <v>15.5</v>
+      </c>
+      <c r="G52" s="1">
+        <v>3.6900000000000003E-198</v>
+      </c>
+      <c r="H52">
+        <v>30.00227117</v>
+      </c>
+    </row>
+    <row r="53" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F53">
+        <v>15.55</v>
+      </c>
+      <c r="G53" s="1">
+        <v>3.1299999999999998E-232</v>
+      </c>
+      <c r="H53">
+        <v>32.511349430000003</v>
+      </c>
+    </row>
+    <row r="54" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F54">
+        <v>15.6</v>
+      </c>
+      <c r="G54" s="1">
+        <v>2.8800000000000001E-110</v>
+      </c>
+      <c r="H54">
+        <v>22.26632639</v>
+      </c>
+    </row>
+    <row r="55" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F55">
+        <v>15.65</v>
+      </c>
+      <c r="G55" s="1">
+        <v>5.1100000000000002E-255</v>
+      </c>
+      <c r="H55">
+        <v>34.084508530000001</v>
+      </c>
+    </row>
+    <row r="56" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F56">
+        <v>15.7</v>
+      </c>
+      <c r="G56">
+        <v>0</v>
+      </c>
+      <c r="H56">
+        <v>38.793739189999997</v>
+      </c>
+    </row>
+    <row r="57" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F57">
+        <v>15.75</v>
+      </c>
+      <c r="G57">
+        <v>0</v>
+      </c>
+      <c r="H57">
+        <v>45.32580875</v>
+      </c>
+    </row>
+    <row r="58" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F58">
+        <v>15.8</v>
+      </c>
+      <c r="G58" s="1">
+        <v>1.4500000000000001E-248</v>
+      </c>
+      <c r="H58">
+        <v>33.646285249999998</v>
+      </c>
+    </row>
+    <row r="59" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F59">
+        <v>15.85</v>
+      </c>
+      <c r="G59">
+        <v>0</v>
+      </c>
+      <c r="H59">
+        <v>41.536072609999998</v>
+      </c>
+    </row>
+    <row r="60" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F60">
+        <v>15.9</v>
+      </c>
+      <c r="G60">
+        <v>0</v>
+      </c>
+      <c r="H60">
+        <v>48.259399620000003</v>
+      </c>
+    </row>
+    <row r="61" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F61">
+        <v>15.95</v>
+      </c>
+      <c r="G61">
+        <v>0</v>
+      </c>
+      <c r="H61">
+        <v>49.901973519999999</v>
+      </c>
+    </row>
+    <row r="62" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F62">
+        <v>16</v>
+      </c>
+      <c r="G62">
+        <v>0</v>
+      </c>
+      <c r="H62">
+        <v>55.178391949999998</v>
+      </c>
+    </row>
+    <row r="63" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F63">
+        <v>16.05</v>
+      </c>
+      <c r="G63">
+        <v>0</v>
+      </c>
+      <c r="H63">
+        <v>45.986240789999997</v>
+      </c>
+    </row>
+    <row r="64" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F64">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="G64">
+        <v>0</v>
+      </c>
+      <c r="H64">
+        <v>46.327086399999999</v>
+      </c>
+    </row>
+    <row r="65" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F65">
+        <v>16.149999999999999</v>
+      </c>
+      <c r="G65">
+        <v>0</v>
+      </c>
+      <c r="H65">
+        <v>51.807381560000003</v>
+      </c>
+    </row>
+    <row r="66" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F66">
+        <v>16.2</v>
+      </c>
+      <c r="G66">
+        <v>0</v>
+      </c>
+      <c r="H66">
+        <v>44.333788630000001</v>
+      </c>
+    </row>
+    <row r="67" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F67">
+        <v>16.25</v>
+      </c>
+      <c r="G67">
+        <v>0</v>
+      </c>
+      <c r="H67">
+        <v>37.786638410000002</v>
+      </c>
+    </row>
+    <row r="68" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F68">
+        <v>16.3</v>
+      </c>
+      <c r="G68" s="1">
+        <v>9.5100000000000004E-94</v>
+      </c>
+      <c r="H68">
+        <v>20.505245630000001</v>
+      </c>
+    </row>
+    <row r="69" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F69">
+        <v>16.350000000000001</v>
+      </c>
+      <c r="G69">
+        <v>0</v>
+      </c>
+      <c r="H69">
+        <v>40.222130829999998</v>
+      </c>
+    </row>
+    <row r="70" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F70">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="G70">
+        <v>0</v>
+      </c>
+      <c r="H70">
+        <v>63.382422339999998</v>
+      </c>
+    </row>
+    <row r="71" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F71">
+        <v>16.45</v>
+      </c>
+      <c r="G71">
+        <v>0</v>
+      </c>
+      <c r="H71">
+        <v>54.431780600000003</v>
+      </c>
+    </row>
+    <row r="72" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F72">
+        <v>16.5</v>
+      </c>
+      <c r="G72" s="1">
+        <v>9.01E-283</v>
+      </c>
+      <c r="H72">
+        <v>35.909150449999999</v>
+      </c>
+    </row>
+    <row r="73" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F73">
+        <v>16.55</v>
+      </c>
+      <c r="G73">
+        <v>0</v>
+      </c>
+      <c r="H73">
+        <v>57.994749759999998</v>
+      </c>
+    </row>
+    <row r="74" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F74">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="G74">
+        <v>0</v>
+      </c>
+      <c r="H74">
+        <v>39.619888799999998</v>
+      </c>
+    </row>
+    <row r="75" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F75">
+        <v>16.649999999999999</v>
+      </c>
+      <c r="G75">
+        <v>0</v>
+      </c>
+      <c r="H75">
+        <v>52.435928769999997</v>
+      </c>
+    </row>
+    <row r="76" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F76">
+        <v>16.7</v>
+      </c>
+      <c r="G76">
+        <v>0</v>
+      </c>
+      <c r="H76">
+        <v>45.991395070000003</v>
+      </c>
+    </row>
+    <row r="77" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F77">
+        <v>16.75</v>
+      </c>
+      <c r="G77">
+        <v>0</v>
+      </c>
+      <c r="H77">
+        <v>60.805634220000002</v>
+      </c>
+    </row>
+    <row r="78" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F78">
+        <v>16.8</v>
+      </c>
+      <c r="G78">
+        <v>0</v>
+      </c>
+      <c r="H78">
+        <v>55.991143950000001</v>
+      </c>
+    </row>
+    <row r="79" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F79">
+        <v>16.850000000000001</v>
+      </c>
+      <c r="G79">
+        <v>0</v>
+      </c>
+      <c r="H79">
+        <v>53.735258520000002</v>
+      </c>
+    </row>
+    <row r="80" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F80">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="G80">
+        <v>0</v>
+      </c>
+      <c r="H80">
+        <v>50.474030370000001</v>
+      </c>
+    </row>
+    <row r="81" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F81">
+        <v>16.95</v>
+      </c>
+      <c r="G81">
+        <v>0</v>
+      </c>
+      <c r="H81">
+        <v>64.902049869999999</v>
+      </c>
+    </row>
+    <row r="82" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F82">
+        <v>17</v>
+      </c>
+      <c r="G82">
+        <v>0</v>
+      </c>
+      <c r="H82">
+        <v>47.123173909999998</v>
+      </c>
+    </row>
+    <row r="83" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F83">
+        <v>17.05</v>
+      </c>
+      <c r="G83">
+        <v>0</v>
+      </c>
+      <c r="H83">
+        <v>62.612712639999998</v>
+      </c>
+    </row>
+    <row r="84" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F84">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="G84">
+        <v>0</v>
+      </c>
+      <c r="H84">
+        <v>45.592973129999997</v>
+      </c>
+    </row>
+    <row r="85" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F85">
+        <v>17.149999999999999</v>
+      </c>
+      <c r="G85">
+        <v>0</v>
+      </c>
+      <c r="H85">
+        <v>57.571889630000001</v>
+      </c>
+    </row>
+    <row r="86" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F86">
+        <v>17.2</v>
+      </c>
+      <c r="G86">
+        <v>0</v>
+      </c>
+      <c r="H86">
+        <v>49.213457560000002</v>
+      </c>
+    </row>
+    <row r="87" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F87">
+        <v>17.25</v>
+      </c>
+      <c r="G87">
+        <v>0</v>
+      </c>
+      <c r="H87">
+        <v>73.310925929999996</v>
+      </c>
+    </row>
+    <row r="88" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F88">
+        <v>17.3</v>
+      </c>
+      <c r="G88">
+        <v>0</v>
+      </c>
+      <c r="H88">
+        <v>53.930424670000001</v>
+      </c>
+    </row>
+    <row r="89" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F89">
+        <v>17.350000000000001</v>
+      </c>
+      <c r="G89">
+        <v>0</v>
+      </c>
+      <c r="H89">
+        <v>39.992796660000003</v>
+      </c>
+    </row>
+    <row r="90" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F90">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="G90">
+        <v>0</v>
+      </c>
+      <c r="H90">
+        <v>46.873295859999999</v>
+      </c>
+    </row>
+    <row r="91" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F91">
+        <v>17.45</v>
+      </c>
+      <c r="G91">
+        <v>0</v>
+      </c>
+      <c r="H91">
+        <v>57.243447670000002</v>
+      </c>
+    </row>
+    <row r="92" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F92">
+        <v>17.5</v>
+      </c>
+      <c r="G92">
+        <v>0</v>
+      </c>
+      <c r="H92">
+        <v>45.329305239999997</v>
+      </c>
+    </row>
+    <row r="93" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F93">
+        <v>17.55</v>
+      </c>
+      <c r="G93">
+        <v>0</v>
+      </c>
+      <c r="H93">
+        <v>66.799228110000001</v>
+      </c>
+    </row>
+    <row r="94" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F94">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="G94">
+        <v>0</v>
+      </c>
+      <c r="H94">
+        <v>65.608590629999995</v>
+      </c>
+    </row>
+    <row r="95" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F95">
+        <v>17.649999999999999</v>
+      </c>
+      <c r="G95">
+        <v>0</v>
+      </c>
+      <c r="H95">
+        <v>59.95183153</v>
+      </c>
+    </row>
+    <row r="96" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F96">
+        <v>17.7</v>
+      </c>
+      <c r="G96" s="1">
+        <v>4.1000000000000001E-261</v>
+      </c>
+      <c r="H96">
+        <v>34.49937224</v>
+      </c>
+    </row>
+    <row r="97" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F97">
+        <v>17.75</v>
+      </c>
+      <c r="G97">
+        <v>0</v>
+      </c>
+      <c r="H97">
+        <v>55.241538570000003</v>
+      </c>
+    </row>
+    <row r="98" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F98">
+        <v>17.8</v>
+      </c>
+      <c r="G98">
+        <v>0</v>
+      </c>
+      <c r="H98">
+        <v>66.491348590000001</v>
+      </c>
+    </row>
+    <row r="99" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F99">
+        <v>17.850000000000001</v>
+      </c>
+      <c r="G99">
+        <v>0</v>
+      </c>
+      <c r="H99">
+        <v>72.221384909999998</v>
+      </c>
+    </row>
+    <row r="100" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F100">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="G100">
+        <v>0</v>
+      </c>
+      <c r="H100">
+        <v>56.89401325</v>
+      </c>
+    </row>
+    <row r="101" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F101">
+        <v>17.95</v>
+      </c>
+      <c r="G101">
+        <v>0</v>
+      </c>
+      <c r="H101">
+        <v>63.383825569999999</v>
+      </c>
+    </row>
+    <row r="102" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F102">
+        <v>18</v>
+      </c>
+      <c r="G102">
+        <v>0</v>
+      </c>
+      <c r="H102">
+        <v>70.318928779999993</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fixed sequence length for Pout=-7 dBm (1024->4096)
</commit_message>
<xml_diff>
--- a/APD+FILT+TIA+LIA.xlsx
+++ b/APD+FILT+TIA+LIA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timur/Desktop/карантин/BERvsQfactor/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF02A6E7-24D4-AB40-8CD2-AE1726229D34}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B354F3E6-74E7-754A-8047-82F6B29C09A2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="14400" windowHeight="8120" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name=" Выходная мощность 3 дБм" sheetId="1" r:id="rId1"/>
@@ -2098,8 +2098,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B3CADCF-C2E9-764E-ADBA-D979EDBEAE38}">
   <dimension ref="A1:L102"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2127,7 +2127,7 @@
         <v>5</v>
       </c>
       <c r="L1">
-        <v>1024</v>
+        <v>4096</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -3457,7 +3457,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D12F1B7-876E-D145-8035-611196C117A8}">
   <dimension ref="A1:L102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:L102"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Noise of LIA = -10 dBm. Jump in BER(OSNR) remains.
</commit_message>
<xml_diff>
--- a/APD+FILT+TIA+LIA.xlsx
+++ b/APD+FILT+TIA+LIA.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timur/Desktop/карантин/BERvsQfactor/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B354F3E6-74E7-754A-8047-82F6B29C09A2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3A793DE-D425-F840-A7FD-7C75079FA30D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19020" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name=" Выходная мощность 3 дБм" sheetId="1" r:id="rId1"/>
     <sheet name="Выходная мощность -7 дБм" sheetId="2" r:id="rId2"/>
     <sheet name="Gain of output ampl = 0" sheetId="3" r:id="rId3"/>
+    <sheet name="Noise Of LIA = -10 dBm" sheetId="6" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="7">
   <si>
     <t>OSNR, dB</t>
   </si>
@@ -103,6 +104,1559 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>BER(OSNR),</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> dB VS dB</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Выходная мощность -7 дБм'!$F$2:$F$102</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="101"/>
+                <c:pt idx="0">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13.05</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13.15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13.25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13.3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>13.35</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>13.4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13.45</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>13.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13.55</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13.6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13.65</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>13.7</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>13.75</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>13.8</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>13.85</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>13.9</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>13.95</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>14.05</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>14.1</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>14.15</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>14.2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>14.25</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>14.3</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>14.35</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>14.4</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>14.45</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>14.5</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>14.55</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>14.6</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>14.65</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>14.7</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>14.75</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>14.8</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>14.85</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>14.9</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>14.95</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>15.05</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>15.1</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>15.15</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>15.2</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>15.25</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>15.3</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>15.35</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>15.4</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>15.45</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>15.5</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>15.55</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>15.6</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>15.65</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>15.7</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>15.75</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>15.8</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>15.85</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>15.9</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>15.95</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>16.05</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>16.100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>16.149999999999999</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>16.2</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>16.25</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>16.3</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>16.350000000000001</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>16.399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>16.45</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>16.5</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>16.55</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>16.600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>16.649999999999999</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>16.7</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>16.75</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>16.8</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>16.850000000000001</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>16.899999999999999</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>16.95</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>17.05</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>17.100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>17.149999999999999</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>17.2</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>17.25</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>17.3</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>17.350000000000001</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>17.399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>17.45</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>17.5</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>17.55</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>17.600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>17.649999999999999</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>17.7</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>17.75</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>17.8</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>17.850000000000001</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>17.899999999999999</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>17.95</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>18</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Выходная мощность -7 дБм'!$I$2:$I$102</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="101"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-999.54677021213342</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>-1077.2584215073632</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>-1077.5448733218584</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>-2052.0620961530917</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>-1000</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>-425.27243550682789</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>-1638.1530856918241</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>-1534.6344155742847</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>-1000</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>-1000</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>-2352.4949160514866</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>-2089.8716277529484</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>-2558.9619627904403</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>-1000</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>-1000</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>-1000</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>-2919.3181413825387</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>-2292.7984069659406</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>-1000</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>-1000</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>-1000</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>-1000</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>-1000</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>-1000</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>-1000</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>-1000</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>-1000</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>-1000</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>-1000</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>-1000</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>-1000</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>-1000</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>-1000</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>-1000</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>-1000</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>-1000</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>-1000</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>-1000</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>-1000</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>-1000</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>-1000</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>-1000</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>-1000</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>-1000</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>-1000</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>-1000</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>-1000</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>-1000</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>-1000</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>-1000</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>-1000</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>-1000</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>-1000</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>-1000</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>-1000</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>-1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-D961-A74E-BC58-70A9C5851EE7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1392552687"/>
+        <c:axId val="1392910431"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1392552687"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="19"/>
+          <c:min val="12"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1392910431"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1392910431"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1392552687"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{40864907-5D00-894C-BCED-48B4B7C9BD15}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2098,8 +3652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B3CADCF-C2E9-764E-ADBA-D979EDBEAE38}">
   <dimension ref="A1:L102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2149,6 +3703,10 @@
       <c r="H2">
         <v>0</v>
       </c>
+      <c r="I2">
+        <f>IF(G2=0, -1000, 10*LOG10(G2))</f>
+        <v>0</v>
+      </c>
       <c r="K2" t="s">
         <v>6</v>
       </c>
@@ -2175,6 +3733,10 @@
       <c r="H3">
         <v>0</v>
       </c>
+      <c r="I3" s="2">
+        <f t="shared" ref="I3:I66" si="0">IF(G3=0, -1000, 10*LOG10(G3))</f>
+        <v>0</v>
+      </c>
       <c r="K3" t="s">
         <v>3</v>
       </c>
@@ -2201,6 +3763,10 @@
       <c r="H4">
         <v>0</v>
       </c>
+      <c r="I4" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="K4" t="s">
         <v>4</v>
       </c>
@@ -2227,6 +3793,10 @@
       <c r="H5">
         <v>0</v>
       </c>
+      <c r="I5" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6">
@@ -2247,6 +3817,10 @@
       <c r="H6">
         <v>0</v>
       </c>
+      <c r="I6" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7">
@@ -2267,6 +3841,10 @@
       <c r="H7">
         <v>0</v>
       </c>
+      <c r="I7" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8">
@@ -2287,6 +3865,10 @@
       <c r="H8">
         <v>0</v>
       </c>
+      <c r="I8" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9">
@@ -2307,6 +3889,10 @@
       <c r="H9">
         <v>0</v>
       </c>
+      <c r="I9" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10">
@@ -2327,6 +3913,10 @@
       <c r="H10">
         <v>0</v>
       </c>
+      <c r="I10" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11">
@@ -2347,6 +3937,10 @@
       <c r="H11">
         <v>0</v>
       </c>
+      <c r="I11" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12">
@@ -2367,6 +3961,10 @@
       <c r="H12">
         <v>0</v>
       </c>
+      <c r="I12" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13">
@@ -2387,6 +3985,10 @@
       <c r="H13">
         <v>0</v>
       </c>
+      <c r="I13" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14">
@@ -2407,6 +4009,10 @@
       <c r="H14">
         <v>0</v>
       </c>
+      <c r="I14" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15">
@@ -2427,6 +4033,10 @@
       <c r="H15">
         <v>0</v>
       </c>
+      <c r="I15" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16">
@@ -2447,8 +4057,12 @@
       <c r="H16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I16" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>25</v>
       </c>
@@ -2467,8 +4081,12 @@
       <c r="H17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I17" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>26</v>
       </c>
@@ -2487,8 +4105,12 @@
       <c r="H18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I18" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>27</v>
       </c>
@@ -2507,8 +4129,12 @@
       <c r="H19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I19" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>28</v>
       </c>
@@ -2527,8 +4153,12 @@
       <c r="H20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I20" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>29</v>
       </c>
@@ -2547,8 +4177,12 @@
       <c r="H21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I21" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>30</v>
       </c>
@@ -2567,8 +4201,12 @@
       <c r="H22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I22" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="F23">
         <v>14.05</v>
       </c>
@@ -2578,8 +4216,12 @@
       <c r="H23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I23" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="F24">
         <v>14.1</v>
       </c>
@@ -2589,8 +4231,12 @@
       <c r="H24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I24" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="F25">
         <v>14.15</v>
       </c>
@@ -2600,8 +4246,12 @@
       <c r="H25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I25" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="F26">
         <v>14.2</v>
       </c>
@@ -2611,8 +4261,12 @@
       <c r="H26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I26" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="F27">
         <v>14.25</v>
       </c>
@@ -2622,8 +4276,12 @@
       <c r="H27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I27" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="F28">
         <v>14.3</v>
       </c>
@@ -2633,8 +4291,12 @@
       <c r="H28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I28" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="F29">
         <v>14.35</v>
       </c>
@@ -2644,8 +4306,12 @@
       <c r="H29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I29" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="F30">
         <v>14.4</v>
       </c>
@@ -2655,8 +4321,12 @@
       <c r="H30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I30" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="F31">
         <v>14.45</v>
       </c>
@@ -2666,8 +4336,12 @@
       <c r="H31">
         <v>21.265233550000001</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I31" s="2">
+        <f t="shared" si="0"/>
+        <v>-999.54677021213342</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="F32">
         <v>14.5</v>
       </c>
@@ -2677,8 +4351,12 @@
       <c r="H32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I32" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F33">
         <v>14.55</v>
       </c>
@@ -2688,8 +4366,12 @@
       <c r="H33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I33" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F34">
         <v>14.6</v>
       </c>
@@ -2699,8 +4381,12 @@
       <c r="H34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I34" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F35">
         <v>14.65</v>
       </c>
@@ -2710,8 +4396,12 @@
       <c r="H35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I35" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F36">
         <v>14.7</v>
       </c>
@@ -2721,8 +4411,12 @@
       <c r="H36">
         <v>22.087569550000001</v>
       </c>
-    </row>
-    <row r="37" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I36" s="2">
+        <f t="shared" si="0"/>
+        <v>-1077.2584215073632</v>
+      </c>
+    </row>
+    <row r="37" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F37">
         <v>14.75</v>
       </c>
@@ -2732,8 +4426,12 @@
       <c r="H37">
         <v>22.085593889999998</v>
       </c>
-    </row>
-    <row r="38" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I37" s="2">
+        <f t="shared" si="0"/>
+        <v>-1077.5448733218584</v>
+      </c>
+    </row>
+    <row r="38" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F38">
         <v>14.8</v>
       </c>
@@ -2743,8 +4441,12 @@
       <c r="H38">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I38" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F39">
         <v>14.85</v>
       </c>
@@ -2754,8 +4456,12 @@
       <c r="H39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I39" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F40">
         <v>14.9</v>
       </c>
@@ -2765,8 +4471,12 @@
       <c r="H40">
         <v>30.592749470000001</v>
       </c>
-    </row>
-    <row r="41" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I40" s="2">
+        <f t="shared" si="0"/>
+        <v>-2052.0620961530917</v>
+      </c>
+    </row>
+    <row r="41" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F41">
         <v>14.95</v>
       </c>
@@ -2776,8 +4486,12 @@
       <c r="H41">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I41" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F42">
         <v>15</v>
       </c>
@@ -2787,8 +4501,12 @@
       <c r="H42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I42" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F43">
         <v>15.05</v>
       </c>
@@ -2798,8 +4516,12 @@
       <c r="H43">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I43" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F44">
         <v>15.1</v>
       </c>
@@ -2809,8 +4531,12 @@
       <c r="H44">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I44" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F45">
         <v>15.15</v>
       </c>
@@ -2820,8 +4546,12 @@
       <c r="H45">
         <v>39.316776590000003</v>
       </c>
-    </row>
-    <row r="46" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I45" s="2">
+        <f t="shared" si="0"/>
+        <v>-1000</v>
+      </c>
+    </row>
+    <row r="46" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F46">
         <v>15.2</v>
       </c>
@@ -2831,8 +4561,12 @@
       <c r="H46">
         <v>13.72634712</v>
       </c>
-    </row>
-    <row r="47" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I46" s="2">
+        <f t="shared" si="0"/>
+        <v>-425.27243550682789</v>
+      </c>
+    </row>
+    <row r="47" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F47">
         <v>15.25</v>
       </c>
@@ -2842,8 +4576,12 @@
       <c r="H47">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I47" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F48">
         <v>15.3</v>
       </c>
@@ -2853,8 +4591,12 @@
       <c r="H48">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I48" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F49">
         <v>15.35</v>
       </c>
@@ -2864,8 +4606,12 @@
       <c r="H49">
         <v>27.310688150000001</v>
       </c>
-    </row>
-    <row r="50" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I49" s="2">
+        <f t="shared" si="0"/>
+        <v>-1638.1530856918241</v>
+      </c>
+    </row>
+    <row r="50" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F50">
         <v>15.4</v>
       </c>
@@ -2875,8 +4621,12 @@
       <c r="H50">
         <v>26.42082826</v>
       </c>
-    </row>
-    <row r="51" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I50" s="2">
+        <f t="shared" si="0"/>
+        <v>-1534.6344155742847</v>
+      </c>
+    </row>
+    <row r="51" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F51">
         <v>15.45</v>
       </c>
@@ -2886,8 +4636,12 @@
       <c r="H51">
         <v>40.48602588</v>
       </c>
-    </row>
-    <row r="52" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I51" s="2">
+        <f t="shared" si="0"/>
+        <v>-1000</v>
+      </c>
+    </row>
+    <row r="52" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F52">
         <v>15.5</v>
       </c>
@@ -2897,8 +4651,12 @@
       <c r="H52">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I52" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F53">
         <v>15.55</v>
       </c>
@@ -2908,8 +4666,12 @@
       <c r="H53">
         <v>38.85373053</v>
       </c>
-    </row>
-    <row r="54" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I53" s="2">
+        <f t="shared" si="0"/>
+        <v>-1000</v>
+      </c>
+    </row>
+    <row r="54" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F54">
         <v>15.6</v>
       </c>
@@ -2919,8 +4681,12 @@
       <c r="H54">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I54" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F55">
         <v>15.65</v>
       </c>
@@ -2930,8 +4696,12 @@
       <c r="H55">
         <v>32.774403270000001</v>
       </c>
-    </row>
-    <row r="56" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I55" s="2">
+        <f t="shared" si="0"/>
+        <v>-2352.4949160514866</v>
+      </c>
+    </row>
+    <row r="56" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F56">
         <v>15.7</v>
       </c>
@@ -2941,8 +4711,12 @@
       <c r="H56">
         <v>30.87977849</v>
       </c>
-    </row>
-    <row r="57" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I56" s="2">
+        <f t="shared" si="0"/>
+        <v>-2089.8716277529484</v>
+      </c>
+    </row>
+    <row r="57" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F57">
         <v>15.75</v>
       </c>
@@ -2952,8 +4726,12 @@
       <c r="H57">
         <v>34.197245649999999</v>
       </c>
-    </row>
-    <row r="58" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I57" s="2">
+        <f t="shared" si="0"/>
+        <v>-2558.9619627904403</v>
+      </c>
+    </row>
+    <row r="58" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F58">
         <v>15.8</v>
       </c>
@@ -2963,8 +4741,12 @@
       <c r="H58">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I58" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F59">
         <v>15.85</v>
       </c>
@@ -2974,8 +4756,12 @@
       <c r="H59">
         <v>40.687379040000003</v>
       </c>
-    </row>
-    <row r="60" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I59" s="2">
+        <f t="shared" si="0"/>
+        <v>-1000</v>
+      </c>
+    </row>
+    <row r="60" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F60">
         <v>15.9</v>
       </c>
@@ -2985,8 +4771,12 @@
       <c r="H60">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I60" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F61">
         <v>15.95</v>
       </c>
@@ -2996,8 +4786,12 @@
       <c r="H61">
         <v>50.276012389999998</v>
       </c>
-    </row>
-    <row r="62" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I61" s="2">
+        <f t="shared" si="0"/>
+        <v>-1000</v>
+      </c>
+    </row>
+    <row r="62" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F62">
         <v>16</v>
       </c>
@@ -3007,8 +4801,12 @@
       <c r="H62">
         <v>40.184062750000002</v>
       </c>
-    </row>
-    <row r="63" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I62" s="2">
+        <f t="shared" si="0"/>
+        <v>-1000</v>
+      </c>
+    </row>
+    <row r="63" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F63">
         <v>16.05</v>
       </c>
@@ -3018,8 +4816,12 @@
       <c r="H63">
         <v>36.540523759999999</v>
       </c>
-    </row>
-    <row r="64" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I63" s="2">
+        <f t="shared" si="0"/>
+        <v>-2919.3181413825387</v>
+      </c>
+    </row>
+    <row r="64" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F64">
         <v>16.100000000000001</v>
       </c>
@@ -3029,8 +4831,12 @@
       <c r="H64">
         <v>32.358304269999998</v>
       </c>
-    </row>
-    <row r="65" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I64" s="2">
+        <f t="shared" si="0"/>
+        <v>-2292.7984069659406</v>
+      </c>
+    </row>
+    <row r="65" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F65">
         <v>16.149999999999999</v>
       </c>
@@ -3040,8 +4846,12 @@
       <c r="H65">
         <v>46.143615660000002</v>
       </c>
-    </row>
-    <row r="66" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I65" s="2">
+        <f t="shared" si="0"/>
+        <v>-1000</v>
+      </c>
+    </row>
+    <row r="66" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F66">
         <v>16.2</v>
       </c>
@@ -3051,8 +4861,12 @@
       <c r="H66">
         <v>48.784062069999997</v>
       </c>
-    </row>
-    <row r="67" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I66" s="2">
+        <f t="shared" si="0"/>
+        <v>-1000</v>
+      </c>
+    </row>
+    <row r="67" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F67">
         <v>16.25</v>
       </c>
@@ -3062,8 +4876,12 @@
       <c r="H67">
         <v>48.321877540000003</v>
       </c>
-    </row>
-    <row r="68" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I67" s="2">
+        <f t="shared" ref="I67:I102" si="1">IF(G67=0, -1000, 10*LOG10(G67))</f>
+        <v>-1000</v>
+      </c>
+    </row>
+    <row r="68" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F68">
         <v>16.3</v>
       </c>
@@ -3073,8 +4891,12 @@
       <c r="H68">
         <v>49.631022489999999</v>
       </c>
-    </row>
-    <row r="69" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I68" s="2">
+        <f t="shared" si="1"/>
+        <v>-1000</v>
+      </c>
+    </row>
+    <row r="69" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F69">
         <v>16.350000000000001</v>
       </c>
@@ -3084,8 +4906,12 @@
       <c r="H69">
         <v>49.468441429999999</v>
       </c>
-    </row>
-    <row r="70" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I69" s="2">
+        <f t="shared" si="1"/>
+        <v>-1000</v>
+      </c>
+    </row>
+    <row r="70" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F70">
         <v>16.399999999999999</v>
       </c>
@@ -3095,8 +4921,12 @@
       <c r="H70">
         <v>52.660545939999999</v>
       </c>
-    </row>
-    <row r="71" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I70" s="2">
+        <f t="shared" si="1"/>
+        <v>-1000</v>
+      </c>
+    </row>
+    <row r="71" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F71">
         <v>16.45</v>
       </c>
@@ -3106,8 +4936,12 @@
       <c r="H71">
         <v>48.46359064</v>
       </c>
-    </row>
-    <row r="72" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I71" s="2">
+        <f t="shared" si="1"/>
+        <v>-1000</v>
+      </c>
+    </row>
+    <row r="72" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F72">
         <v>16.5</v>
       </c>
@@ -3117,8 +4951,12 @@
       <c r="H72">
         <v>50.266107259999998</v>
       </c>
-    </row>
-    <row r="73" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I72" s="2">
+        <f t="shared" si="1"/>
+        <v>-1000</v>
+      </c>
+    </row>
+    <row r="73" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F73">
         <v>16.55</v>
       </c>
@@ -3128,8 +4966,12 @@
       <c r="H73">
         <v>49.301880369999999</v>
       </c>
-    </row>
-    <row r="74" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I73" s="2">
+        <f t="shared" si="1"/>
+        <v>-1000</v>
+      </c>
+    </row>
+    <row r="74" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F74">
         <v>16.600000000000001</v>
       </c>
@@ -3139,8 +4981,12 @@
       <c r="H74">
         <v>54.586823500000001</v>
       </c>
-    </row>
-    <row r="75" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I74" s="2">
+        <f t="shared" si="1"/>
+        <v>-1000</v>
+      </c>
+    </row>
+    <row r="75" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F75">
         <v>16.649999999999999</v>
       </c>
@@ -3150,8 +4996,12 @@
       <c r="H75">
         <v>56.198574569999998</v>
       </c>
-    </row>
-    <row r="76" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I75" s="2">
+        <f t="shared" si="1"/>
+        <v>-1000</v>
+      </c>
+    </row>
+    <row r="76" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F76">
         <v>16.7</v>
       </c>
@@ -3161,8 +5011,12 @@
       <c r="H76">
         <v>48.004052420000001</v>
       </c>
-    </row>
-    <row r="77" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I76" s="2">
+        <f t="shared" si="1"/>
+        <v>-1000</v>
+      </c>
+    </row>
+    <row r="77" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F77">
         <v>16.75</v>
       </c>
@@ -3172,8 +5026,12 @@
       <c r="H77">
         <v>57.658728979999999</v>
       </c>
-    </row>
-    <row r="78" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I77" s="2">
+        <f t="shared" si="1"/>
+        <v>-1000</v>
+      </c>
+    </row>
+    <row r="78" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F78">
         <v>16.8</v>
       </c>
@@ -3183,8 +5041,12 @@
       <c r="H78">
         <v>55.133515600000003</v>
       </c>
-    </row>
-    <row r="79" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I78" s="2">
+        <f t="shared" si="1"/>
+        <v>-1000</v>
+      </c>
+    </row>
+    <row r="79" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F79">
         <v>16.850000000000001</v>
       </c>
@@ -3194,8 +5056,12 @@
       <c r="H79">
         <v>54.759498260000001</v>
       </c>
-    </row>
-    <row r="80" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I79" s="2">
+        <f t="shared" si="1"/>
+        <v>-1000</v>
+      </c>
+    </row>
+    <row r="80" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F80">
         <v>16.899999999999999</v>
       </c>
@@ -3205,8 +5071,12 @@
       <c r="H80">
         <v>56.173744980000002</v>
       </c>
-    </row>
-    <row r="81" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I80" s="2">
+        <f t="shared" si="1"/>
+        <v>-1000</v>
+      </c>
+    </row>
+    <row r="81" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F81">
         <v>16.95</v>
       </c>
@@ -3216,8 +5086,12 @@
       <c r="H81">
         <v>61.166705929999999</v>
       </c>
-    </row>
-    <row r="82" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I81" s="2">
+        <f t="shared" si="1"/>
+        <v>-1000</v>
+      </c>
+    </row>
+    <row r="82" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F82">
         <v>17</v>
       </c>
@@ -3227,8 +5101,12 @@
       <c r="H82">
         <v>58.002330290000003</v>
       </c>
-    </row>
-    <row r="83" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I82" s="2">
+        <f t="shared" si="1"/>
+        <v>-1000</v>
+      </c>
+    </row>
+    <row r="83" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F83">
         <v>17.05</v>
       </c>
@@ -3238,8 +5116,12 @@
       <c r="H83">
         <v>51.670730460000001</v>
       </c>
-    </row>
-    <row r="84" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I83" s="2">
+        <f t="shared" si="1"/>
+        <v>-1000</v>
+      </c>
+    </row>
+    <row r="84" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F84">
         <v>17.100000000000001</v>
       </c>
@@ -3249,8 +5131,12 @@
       <c r="H84">
         <v>53.79423895</v>
       </c>
-    </row>
-    <row r="85" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I84" s="2">
+        <f t="shared" si="1"/>
+        <v>-1000</v>
+      </c>
+    </row>
+    <row r="85" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F85">
         <v>17.149999999999999</v>
       </c>
@@ -3260,8 +5146,12 @@
       <c r="H85">
         <v>62.20640968</v>
       </c>
-    </row>
-    <row r="86" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I85" s="2">
+        <f t="shared" si="1"/>
+        <v>-1000</v>
+      </c>
+    </row>
+    <row r="86" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F86">
         <v>17.2</v>
       </c>
@@ -3271,8 +5161,12 @@
       <c r="H86">
         <v>62.61363283</v>
       </c>
-    </row>
-    <row r="87" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I86" s="2">
+        <f t="shared" si="1"/>
+        <v>-1000</v>
+      </c>
+    </row>
+    <row r="87" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F87">
         <v>17.25</v>
       </c>
@@ -3282,8 +5176,12 @@
       <c r="H87">
         <v>63.690048509999997</v>
       </c>
-    </row>
-    <row r="88" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I87" s="2">
+        <f t="shared" si="1"/>
+        <v>-1000</v>
+      </c>
+    </row>
+    <row r="88" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F88">
         <v>17.3</v>
       </c>
@@ -3293,8 +5191,12 @@
       <c r="H88">
         <v>47.30045527</v>
       </c>
-    </row>
-    <row r="89" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I88" s="2">
+        <f t="shared" si="1"/>
+        <v>-1000</v>
+      </c>
+    </row>
+    <row r="89" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F89">
         <v>17.350000000000001</v>
       </c>
@@ -3304,8 +5206,12 @@
       <c r="H89">
         <v>58.132979720000002</v>
       </c>
-    </row>
-    <row r="90" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I89" s="2">
+        <f t="shared" si="1"/>
+        <v>-1000</v>
+      </c>
+    </row>
+    <row r="90" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F90">
         <v>17.399999999999999</v>
       </c>
@@ -3315,8 +5221,12 @@
       <c r="H90">
         <v>57.941216750000002</v>
       </c>
-    </row>
-    <row r="91" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I90" s="2">
+        <f t="shared" si="1"/>
+        <v>-1000</v>
+      </c>
+    </row>
+    <row r="91" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F91">
         <v>17.45</v>
       </c>
@@ -3326,8 +5236,12 @@
       <c r="H91">
         <v>58.118236099999997</v>
       </c>
-    </row>
-    <row r="92" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I91" s="2">
+        <f t="shared" si="1"/>
+        <v>-1000</v>
+      </c>
+    </row>
+    <row r="92" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F92">
         <v>17.5</v>
       </c>
@@ -3337,8 +5251,12 @@
       <c r="H92">
         <v>56.37006178</v>
       </c>
-    </row>
-    <row r="93" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I92" s="2">
+        <f t="shared" si="1"/>
+        <v>-1000</v>
+      </c>
+    </row>
+    <row r="93" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F93">
         <v>17.55</v>
       </c>
@@ -3348,8 +5266,12 @@
       <c r="H93">
         <v>65.745433449999993</v>
       </c>
-    </row>
-    <row r="94" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I93" s="2">
+        <f t="shared" si="1"/>
+        <v>-1000</v>
+      </c>
+    </row>
+    <row r="94" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F94">
         <v>17.600000000000001</v>
       </c>
@@ -3359,8 +5281,12 @@
       <c r="H94">
         <v>64.373812709999996</v>
       </c>
-    </row>
-    <row r="95" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I94" s="2">
+        <f t="shared" si="1"/>
+        <v>-1000</v>
+      </c>
+    </row>
+    <row r="95" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F95">
         <v>17.649999999999999</v>
       </c>
@@ -3370,8 +5296,12 @@
       <c r="H95">
         <v>63.078113960000003</v>
       </c>
-    </row>
-    <row r="96" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I95" s="2">
+        <f t="shared" si="1"/>
+        <v>-1000</v>
+      </c>
+    </row>
+    <row r="96" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F96">
         <v>17.7</v>
       </c>
@@ -3381,8 +5311,12 @@
       <c r="H96">
         <v>63.403778580000001</v>
       </c>
-    </row>
-    <row r="97" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I96" s="2">
+        <f t="shared" si="1"/>
+        <v>-1000</v>
+      </c>
+    </row>
+    <row r="97" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F97">
         <v>17.75</v>
       </c>
@@ -3392,8 +5326,12 @@
       <c r="H97">
         <v>69.787713010000004</v>
       </c>
-    </row>
-    <row r="98" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I97" s="2">
+        <f t="shared" si="1"/>
+        <v>-1000</v>
+      </c>
+    </row>
+    <row r="98" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F98">
         <v>17.8</v>
       </c>
@@ -3403,8 +5341,12 @@
       <c r="H98">
         <v>59.474370010000001</v>
       </c>
-    </row>
-    <row r="99" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I98" s="2">
+        <f t="shared" si="1"/>
+        <v>-1000</v>
+      </c>
+    </row>
+    <row r="99" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F99">
         <v>17.850000000000001</v>
       </c>
@@ -3414,8 +5356,12 @@
       <c r="H99">
         <v>57.372991579999997</v>
       </c>
-    </row>
-    <row r="100" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I99" s="2">
+        <f t="shared" si="1"/>
+        <v>-1000</v>
+      </c>
+    </row>
+    <row r="100" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F100">
         <v>17.899999999999999</v>
       </c>
@@ -3425,8 +5371,12 @@
       <c r="H100">
         <v>67.558118289999996</v>
       </c>
-    </row>
-    <row r="101" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I100" s="2">
+        <f t="shared" si="1"/>
+        <v>-1000</v>
+      </c>
+    </row>
+    <row r="101" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F101">
         <v>17.95</v>
       </c>
@@ -3436,8 +5386,12 @@
       <c r="H101">
         <v>65.243549740000006</v>
       </c>
-    </row>
-    <row r="102" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I101" s="2">
+        <f t="shared" si="1"/>
+        <v>-1000</v>
+      </c>
+    </row>
+    <row r="102" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F102">
         <v>18</v>
       </c>
@@ -3447,9 +5401,14 @@
       <c r="H102">
         <v>64.305960569999996</v>
       </c>
+      <c r="I102" s="2">
+        <f t="shared" si="1"/>
+        <v>-1000</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4810,4 +6769,1363 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A52F5D34-43C1-134A-AB80-DCD47AE19FBC}">
+  <dimension ref="A1:L102"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>13</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="K2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>13.05</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="K3" t="s">
+        <v>3</v>
+      </c>
+      <c r="L3">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>13.1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="K4" t="s">
+        <v>4</v>
+      </c>
+      <c r="L4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>13.15</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>14</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>13.2</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>13.25</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>16</v>
+      </c>
+      <c r="B8" s="1">
+        <v>2.1399999999999999E-89</v>
+      </c>
+      <c r="C8">
+        <v>20.010761989999999</v>
+      </c>
+      <c r="F8">
+        <v>13.3</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>17</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1.49E-68</v>
+      </c>
+      <c r="C9">
+        <v>17.45455316</v>
+      </c>
+      <c r="F9">
+        <v>13.35</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>18</v>
+      </c>
+      <c r="B10" s="1">
+        <v>8.4699999999999997E-91</v>
+      </c>
+      <c r="C10">
+        <v>20.171666030000001</v>
+      </c>
+      <c r="F10">
+        <v>13.4</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>19</v>
+      </c>
+      <c r="B11" s="1">
+        <v>2.6700000000000002E-123</v>
+      </c>
+      <c r="C11">
+        <v>23.585745790000001</v>
+      </c>
+      <c r="F11">
+        <v>13.45</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>20</v>
+      </c>
+      <c r="B12" s="1">
+        <v>2.9799999999999999E-123</v>
+      </c>
+      <c r="C12">
+        <v>23.581459410000001</v>
+      </c>
+      <c r="F12">
+        <v>13.5</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>21</v>
+      </c>
+      <c r="B13" s="1">
+        <v>2.9699999999999998E-134</v>
+      </c>
+      <c r="C13">
+        <v>24.63057714</v>
+      </c>
+      <c r="F13">
+        <v>13.55</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>22</v>
+      </c>
+      <c r="B14" s="1">
+        <v>7.3199999999999998E-132</v>
+      </c>
+      <c r="C14">
+        <v>24.406147740000002</v>
+      </c>
+      <c r="F14">
+        <v>13.6</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>23</v>
+      </c>
+      <c r="B15" s="1">
+        <v>3.1E-145</v>
+      </c>
+      <c r="C15">
+        <v>25.634964350000001</v>
+      </c>
+      <c r="F15">
+        <v>13.65</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>24</v>
+      </c>
+      <c r="B16" s="1">
+        <v>9.8000000000000004E-130</v>
+      </c>
+      <c r="C16">
+        <v>24.205080710000001</v>
+      </c>
+      <c r="F16">
+        <v>13.7</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>25</v>
+      </c>
+      <c r="B17" s="1">
+        <v>2.34E-144</v>
+      </c>
+      <c r="C17">
+        <v>25.556115640000002</v>
+      </c>
+      <c r="F17">
+        <v>13.75</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>26</v>
+      </c>
+      <c r="B18" s="1">
+        <v>6.5900000000000003E-141</v>
+      </c>
+      <c r="C18">
+        <v>25.24394392</v>
+      </c>
+      <c r="F18">
+        <v>13.8</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>27</v>
+      </c>
+      <c r="B19" s="1">
+        <v>1.06E-132</v>
+      </c>
+      <c r="C19">
+        <v>24.485061640000001</v>
+      </c>
+      <c r="F19">
+        <v>13.85</v>
+      </c>
+      <c r="G19" s="1">
+        <v>1.2453E-27</v>
+      </c>
+      <c r="H19">
+        <v>10.820241299999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>28</v>
+      </c>
+      <c r="B20" s="1">
+        <v>1.5700000000000001E-137</v>
+      </c>
+      <c r="C20">
+        <v>24.9343355</v>
+      </c>
+      <c r="F20">
+        <v>13.9</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>29</v>
+      </c>
+      <c r="B21" s="1">
+        <v>3.3599999999999999E-144</v>
+      </c>
+      <c r="C21">
+        <v>25.54210849</v>
+      </c>
+      <c r="F21">
+        <v>13.95</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>30</v>
+      </c>
+      <c r="B22" s="1">
+        <v>1.4000000000000001E-140</v>
+      </c>
+      <c r="C22">
+        <v>25.21407898</v>
+      </c>
+      <c r="F22">
+        <v>14</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F23">
+        <v>14.05</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F24">
+        <v>14.1</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F25">
+        <v>14.15</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F26">
+        <v>14.2</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F27">
+        <v>14.25</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F28">
+        <v>14.3</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F29">
+        <v>14.35</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F30">
+        <v>14.4</v>
+      </c>
+      <c r="G30">
+        <v>1</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F31">
+        <v>14.45</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F32">
+        <v>14.5</v>
+      </c>
+      <c r="G32" s="1">
+        <v>8.8995200000000001E-41</v>
+      </c>
+      <c r="H32">
+        <v>13.315125009999999</v>
+      </c>
+    </row>
+    <row r="33" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F33">
+        <v>14.55</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F34">
+        <v>14.6</v>
+      </c>
+      <c r="G34" s="1">
+        <v>2.31886E-33</v>
+      </c>
+      <c r="H34">
+        <v>11.97774969</v>
+      </c>
+    </row>
+    <row r="35" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F35">
+        <v>14.65</v>
+      </c>
+      <c r="G35">
+        <v>1</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F36">
+        <v>14.7</v>
+      </c>
+      <c r="G36">
+        <v>1</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F37">
+        <v>14.75</v>
+      </c>
+      <c r="G37">
+        <v>1</v>
+      </c>
+      <c r="H37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F38">
+        <v>14.8</v>
+      </c>
+      <c r="G38">
+        <v>1</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F39">
+        <v>14.85</v>
+      </c>
+      <c r="G39">
+        <v>1</v>
+      </c>
+      <c r="H39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F40">
+        <v>14.9</v>
+      </c>
+      <c r="G40">
+        <v>1</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F41">
+        <v>14.95</v>
+      </c>
+      <c r="G41" s="1">
+        <v>1.0331299999999999E-45</v>
+      </c>
+      <c r="H41">
+        <v>14.139075399999999</v>
+      </c>
+    </row>
+    <row r="42" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F42">
+        <v>15</v>
+      </c>
+      <c r="G42" s="1">
+        <v>1.66116E-28</v>
+      </c>
+      <c r="H42">
+        <v>11.00638221</v>
+      </c>
+    </row>
+    <row r="43" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F43">
+        <v>15.05</v>
+      </c>
+      <c r="G43">
+        <v>1</v>
+      </c>
+      <c r="H43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F44">
+        <v>15.1</v>
+      </c>
+      <c r="G44">
+        <v>1</v>
+      </c>
+      <c r="H44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F45">
+        <v>15.15</v>
+      </c>
+      <c r="G45" s="1">
+        <v>2.7595599999999998E-29</v>
+      </c>
+      <c r="H45">
+        <v>11.15887682</v>
+      </c>
+    </row>
+    <row r="46" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F46">
+        <v>15.2</v>
+      </c>
+      <c r="G46">
+        <v>1</v>
+      </c>
+      <c r="H46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F47">
+        <v>15.25</v>
+      </c>
+      <c r="G47" s="1">
+        <v>9.4350300000000007E-52</v>
+      </c>
+      <c r="H47">
+        <v>15.0831103</v>
+      </c>
+    </row>
+    <row r="48" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F48">
+        <v>15.3</v>
+      </c>
+      <c r="G48" s="1">
+        <v>5.3239300000000002E-31</v>
+      </c>
+      <c r="H48">
+        <v>11.518175729999999</v>
+      </c>
+    </row>
+    <row r="49" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F49">
+        <v>15.35</v>
+      </c>
+      <c r="G49">
+        <v>1</v>
+      </c>
+      <c r="H49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F50">
+        <v>15.4</v>
+      </c>
+      <c r="G50">
+        <v>1</v>
+      </c>
+      <c r="H50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F51">
+        <v>15.45</v>
+      </c>
+      <c r="G51">
+        <v>1</v>
+      </c>
+      <c r="H51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F52">
+        <v>15.5</v>
+      </c>
+      <c r="G52">
+        <v>1</v>
+      </c>
+      <c r="H52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F53">
+        <v>15.55</v>
+      </c>
+      <c r="G53" s="1">
+        <v>4.3967100000000004E-53</v>
+      </c>
+      <c r="H53">
+        <v>15.28817841</v>
+      </c>
+    </row>
+    <row r="54" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F54">
+        <v>15.6</v>
+      </c>
+      <c r="G54">
+        <v>1</v>
+      </c>
+      <c r="H54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F55">
+        <v>15.65</v>
+      </c>
+      <c r="G55">
+        <v>1</v>
+      </c>
+      <c r="H55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F56">
+        <v>15.7</v>
+      </c>
+      <c r="G56">
+        <v>1</v>
+      </c>
+      <c r="H56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F57">
+        <v>15.75</v>
+      </c>
+      <c r="G57" s="1">
+        <v>1.35586E-55</v>
+      </c>
+      <c r="H57">
+        <v>15.656054129999999</v>
+      </c>
+    </row>
+    <row r="58" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F58">
+        <v>15.8</v>
+      </c>
+      <c r="G58" s="1">
+        <v>2.1482099999999999E-51</v>
+      </c>
+      <c r="H58">
+        <v>15.03452265</v>
+      </c>
+    </row>
+    <row r="59" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F59">
+        <v>15.85</v>
+      </c>
+      <c r="G59" s="1">
+        <v>1.04975E-29</v>
+      </c>
+      <c r="H59">
+        <v>11.246566550000001</v>
+      </c>
+    </row>
+    <row r="60" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F60">
+        <v>15.9</v>
+      </c>
+      <c r="G60" s="1">
+        <v>4.2830099999999998E-58</v>
+      </c>
+      <c r="H60">
+        <v>16.018773029999998</v>
+      </c>
+    </row>
+    <row r="61" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F61">
+        <v>15.95</v>
+      </c>
+      <c r="G61" s="1">
+        <v>4.9487300000000002E-78</v>
+      </c>
+      <c r="H61">
+        <v>18.662487559999999</v>
+      </c>
+    </row>
+    <row r="62" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F62">
+        <v>16</v>
+      </c>
+      <c r="G62" s="1">
+        <v>4.2213999999999996E-65</v>
+      </c>
+      <c r="H62">
+        <v>16.994692570000002</v>
+      </c>
+    </row>
+    <row r="63" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F63">
+        <v>16.05</v>
+      </c>
+      <c r="G63" s="1">
+        <v>1.8614399999999999E-37</v>
+      </c>
+      <c r="H63">
+        <v>12.730924140000001</v>
+      </c>
+    </row>
+    <row r="64" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F64">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="G64">
+        <v>1</v>
+      </c>
+      <c r="H64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F65">
+        <v>16.149999999999999</v>
+      </c>
+      <c r="G65" s="1">
+        <v>1.2265499999999999E-88</v>
+      </c>
+      <c r="H65">
+        <v>19.924722209999999</v>
+      </c>
+    </row>
+    <row r="66" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F66">
+        <v>16.2</v>
+      </c>
+      <c r="G66">
+        <v>1</v>
+      </c>
+      <c r="H66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F67">
+        <v>16.25</v>
+      </c>
+      <c r="G67">
+        <v>1</v>
+      </c>
+      <c r="H67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F68">
+        <v>16.3</v>
+      </c>
+      <c r="G68" s="1">
+        <v>6.9873999999999999E-49</v>
+      </c>
+      <c r="H68">
+        <v>14.63893266</v>
+      </c>
+    </row>
+    <row r="69" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F69">
+        <v>16.350000000000001</v>
+      </c>
+      <c r="G69" s="1">
+        <v>5.96954E-64</v>
+      </c>
+      <c r="H69">
+        <v>16.83712104</v>
+      </c>
+    </row>
+    <row r="70" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F70">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="G70" s="1">
+        <v>6.5663300000000002E-43</v>
+      </c>
+      <c r="H70">
+        <v>13.678699910000001</v>
+      </c>
+    </row>
+    <row r="71" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F71">
+        <v>16.45</v>
+      </c>
+      <c r="G71">
+        <v>1</v>
+      </c>
+      <c r="H71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F72">
+        <v>16.5</v>
+      </c>
+      <c r="G72" s="1">
+        <v>2.7274500000000001E-51</v>
+      </c>
+      <c r="H72">
+        <v>15.01720253</v>
+      </c>
+    </row>
+    <row r="73" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F73">
+        <v>16.55</v>
+      </c>
+      <c r="G73" s="1">
+        <v>7.8972799999999993E-89</v>
+      </c>
+      <c r="H73">
+        <v>19.94618011</v>
+      </c>
+    </row>
+    <row r="74" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F74">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="G74" s="1">
+        <v>1.3516299999999999E-59</v>
+      </c>
+      <c r="H74">
+        <v>16.23235554</v>
+      </c>
+    </row>
+    <row r="75" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F75">
+        <v>16.649999999999999</v>
+      </c>
+      <c r="G75" s="1">
+        <v>5.1187499999999996E-57</v>
+      </c>
+      <c r="H75">
+        <v>15.864172310000001</v>
+      </c>
+    </row>
+    <row r="76" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F76">
+        <v>16.7</v>
+      </c>
+      <c r="G76" s="1">
+        <v>3.3829699999999998E-59</v>
+      </c>
+      <c r="H76">
+        <v>16.181766459999999</v>
+      </c>
+    </row>
+    <row r="77" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F77">
+        <v>16.75</v>
+      </c>
+      <c r="G77" s="1">
+        <v>2.2365300000000001E-57</v>
+      </c>
+      <c r="H77">
+        <v>15.92179814</v>
+      </c>
+    </row>
+    <row r="78" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F78">
+        <v>16.8</v>
+      </c>
+      <c r="G78" s="1">
+        <v>1.6026200000000001E-55</v>
+      </c>
+      <c r="H78">
+        <v>15.651935569999999</v>
+      </c>
+    </row>
+    <row r="79" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F79">
+        <v>16.850000000000001</v>
+      </c>
+      <c r="G79" s="1">
+        <v>6.6092000000000002E-115</v>
+      </c>
+      <c r="H79">
+        <v>22.75310022</v>
+      </c>
+    </row>
+    <row r="80" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F80">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="G80" s="1">
+        <v>6.1575000000000004E-104</v>
+      </c>
+      <c r="H80">
+        <v>21.616759429999998</v>
+      </c>
+    </row>
+    <row r="81" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F81">
+        <v>16.95</v>
+      </c>
+      <c r="G81" s="1">
+        <v>4.6369E-91</v>
+      </c>
+      <c r="H81">
+        <v>20.202354029999999</v>
+      </c>
+    </row>
+    <row r="82" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F82">
+        <v>17</v>
+      </c>
+      <c r="G82" s="1">
+        <v>8.0177099999999997E-62</v>
+      </c>
+      <c r="H82">
+        <v>16.548165829999999</v>
+      </c>
+    </row>
+    <row r="83" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F83">
+        <v>17.05</v>
+      </c>
+      <c r="G83" s="1">
+        <v>2.8458900000000001E-62</v>
+      </c>
+      <c r="H83">
+        <v>16.612121940000002</v>
+      </c>
+    </row>
+    <row r="84" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F84">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="G84" s="1">
+        <v>2.9988499999999999E-85</v>
+      </c>
+      <c r="H84">
+        <v>19.53081637</v>
+      </c>
+    </row>
+    <row r="85" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F85">
+        <v>17.149999999999999</v>
+      </c>
+      <c r="G85" s="1">
+        <v>1.66701E-74</v>
+      </c>
+      <c r="H85">
+        <v>18.223839130000002</v>
+      </c>
+    </row>
+    <row r="86" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F86">
+        <v>17.2</v>
+      </c>
+      <c r="G86" s="1">
+        <v>8.2317500000000004E-86</v>
+      </c>
+      <c r="H86">
+        <v>19.595290070000001</v>
+      </c>
+    </row>
+    <row r="87" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F87">
+        <v>17.25</v>
+      </c>
+      <c r="G87">
+        <v>1</v>
+      </c>
+      <c r="H87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F88">
+        <v>17.3</v>
+      </c>
+      <c r="G88" s="1">
+        <v>5.3688599999999997E-68</v>
+      </c>
+      <c r="H88">
+        <v>17.382629300000001</v>
+      </c>
+    </row>
+    <row r="89" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F89">
+        <v>17.350000000000001</v>
+      </c>
+      <c r="G89" s="1">
+        <v>3.0497899999999999E-98</v>
+      </c>
+      <c r="H89">
+        <v>21.003417689999999</v>
+      </c>
+    </row>
+    <row r="90" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F90">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="G90" s="1">
+        <v>4.4483400000000001E-42</v>
+      </c>
+      <c r="H90">
+        <v>13.532856560000001</v>
+      </c>
+    </row>
+    <row r="91" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F91">
+        <v>17.45</v>
+      </c>
+      <c r="G91" s="1">
+        <v>2.62757E-93</v>
+      </c>
+      <c r="H91">
+        <v>20.456432289999999</v>
+      </c>
+    </row>
+    <row r="92" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F92">
+        <v>17.5</v>
+      </c>
+      <c r="G92" s="1">
+        <v>4.2565700000000003E-93</v>
+      </c>
+      <c r="H92">
+        <v>20.43292344</v>
+      </c>
+    </row>
+    <row r="93" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F93">
+        <v>17.55</v>
+      </c>
+      <c r="G93" s="1">
+        <v>7.7884099999999998E-56</v>
+      </c>
+      <c r="H93">
+        <v>15.691938110000001</v>
+      </c>
+    </row>
+    <row r="94" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F94">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="G94" s="1">
+        <v>2.17824E-41</v>
+      </c>
+      <c r="H94">
+        <v>13.424268939999999</v>
+      </c>
+    </row>
+    <row r="95" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F95">
+        <v>17.649999999999999</v>
+      </c>
+      <c r="G95" s="1">
+        <v>8.6774000000000005E-99</v>
+      </c>
+      <c r="H95">
+        <v>21.061680819999999</v>
+      </c>
+    </row>
+    <row r="96" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F96">
+        <v>17.7</v>
+      </c>
+      <c r="G96" s="1">
+        <v>9.7083999999999997E-123</v>
+      </c>
+      <c r="H96">
+        <v>23.530700750000001</v>
+      </c>
+    </row>
+    <row r="97" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F97">
+        <v>17.75</v>
+      </c>
+      <c r="G97" s="1">
+        <v>2.64633E-93</v>
+      </c>
+      <c r="H97">
+        <v>20.454875850000001</v>
+      </c>
+    </row>
+    <row r="98" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F98">
+        <v>17.8</v>
+      </c>
+      <c r="G98" s="1">
+        <v>8.0738999999999998E-108</v>
+      </c>
+      <c r="H98">
+        <v>22.02499877</v>
+      </c>
+    </row>
+    <row r="99" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F99">
+        <v>17.850000000000001</v>
+      </c>
+      <c r="G99" s="1">
+        <v>3.91942E-22</v>
+      </c>
+      <c r="H99">
+        <v>9.5885448610000008</v>
+      </c>
+    </row>
+    <row r="100" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F100">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="G100" s="1">
+        <v>8.7622399999999994E-68</v>
+      </c>
+      <c r="H100">
+        <v>17.353835539999999</v>
+      </c>
+    </row>
+    <row r="101" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F101">
+        <v>17.95</v>
+      </c>
+      <c r="G101" s="1">
+        <v>7.7811699999999993E-71</v>
+      </c>
+      <c r="H101">
+        <v>17.752601890000001</v>
+      </c>
+    </row>
+    <row r="102" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F102">
+        <v>18</v>
+      </c>
+      <c r="G102" s="1">
+        <v>1.3471E-129</v>
+      </c>
+      <c r="H102">
+        <v>24.191987260000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Noise of LIA = -5 dBm. Jump in BER(OSNR) remains
</commit_message>
<xml_diff>
--- a/APD+FILT+TIA+LIA.xlsx
+++ b/APD+FILT+TIA+LIA.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timur/Desktop/карантин/BERvsQfactor/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3A793DE-D425-F840-A7FD-7C75079FA30D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F91A3194-9372-4147-B30E-F05BA7EE1FD8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19020" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19020" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name=" Выходная мощность 3 дБм" sheetId="1" r:id="rId1"/>
     <sheet name="Выходная мощность -7 дБм" sheetId="2" r:id="rId2"/>
     <sheet name="Gain of output ampl = 0" sheetId="3" r:id="rId3"/>
     <sheet name="Noise Of LIA = -10 dBm" sheetId="6" r:id="rId4"/>
+    <sheet name="Noise Of LIA = -5 dBm" sheetId="8" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="7">
   <si>
     <t>OSNR, dB</t>
   </si>
@@ -6775,7 +6776,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A52F5D34-43C1-134A-AB80-DCD47AE19FBC}">
   <dimension ref="A1:L102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
@@ -8128,4 +8129,813 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16811C81-6436-6A4A-8EB7-EDFDF19EEB49}">
+  <dimension ref="A1:L52"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:L52"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>13</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="K2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>13.1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="K3" t="s">
+        <v>3</v>
+      </c>
+      <c r="L3">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>13.2</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="K4" t="s">
+        <v>4</v>
+      </c>
+      <c r="L4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>13.3</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>14</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>13.4</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>13.5</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>16</v>
+      </c>
+      <c r="B8" s="1">
+        <v>9.4100000000000005E-40</v>
+      </c>
+      <c r="C8">
+        <v>13.14233522</v>
+      </c>
+      <c r="F8">
+        <v>13.6</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>17</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1.5000000000000001E-33</v>
+      </c>
+      <c r="C9">
+        <v>12.011796390000001</v>
+      </c>
+      <c r="F9">
+        <v>13.7</v>
+      </c>
+      <c r="G9" s="1">
+        <v>3.2699999999999999E-18</v>
+      </c>
+      <c r="H9">
+        <v>8.6199083549999997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>18</v>
+      </c>
+      <c r="B10" s="1">
+        <v>4.34E-38</v>
+      </c>
+      <c r="C10">
+        <v>12.84780617</v>
+      </c>
+      <c r="F10">
+        <v>13.8</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>19</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1.79E-43</v>
+      </c>
+      <c r="C11">
+        <v>13.77531804</v>
+      </c>
+      <c r="F11">
+        <v>13.9</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>20</v>
+      </c>
+      <c r="B12" s="1">
+        <v>6.9099999999999998E-46</v>
+      </c>
+      <c r="C12">
+        <v>14.171127439999999</v>
+      </c>
+      <c r="F12">
+        <v>14</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>21</v>
+      </c>
+      <c r="B13" s="1">
+        <v>3.5499999999999997E-46</v>
+      </c>
+      <c r="C13">
+        <v>14.217695770000001</v>
+      </c>
+      <c r="F13">
+        <v>14.1</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>22</v>
+      </c>
+      <c r="B14" s="1">
+        <v>8.0999999999999994E-48</v>
+      </c>
+      <c r="C14">
+        <v>14.47999132</v>
+      </c>
+      <c r="F14">
+        <v>14.2</v>
+      </c>
+      <c r="G14" s="1">
+        <v>1.4999999999999999E-18</v>
+      </c>
+      <c r="H14">
+        <v>8.7082435740000008</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>23</v>
+      </c>
+      <c r="B15" s="1">
+        <v>2.1900000000000002E-47</v>
+      </c>
+      <c r="C15">
+        <v>14.41125551</v>
+      </c>
+      <c r="F15">
+        <v>14.3</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>24</v>
+      </c>
+      <c r="B16" s="1">
+        <v>2.51E-46</v>
+      </c>
+      <c r="C16">
+        <v>14.241918310000001</v>
+      </c>
+      <c r="F16">
+        <v>14.4</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>25</v>
+      </c>
+      <c r="B17" s="1">
+        <v>7.1099999999999997E-47</v>
+      </c>
+      <c r="C17">
+        <v>14.32965224</v>
+      </c>
+      <c r="F17">
+        <v>14.5</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>26</v>
+      </c>
+      <c r="B18" s="1">
+        <v>4.2300000000000003E-48</v>
+      </c>
+      <c r="C18">
+        <v>14.52442797</v>
+      </c>
+      <c r="F18">
+        <v>14.6</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>27</v>
+      </c>
+      <c r="B19" s="1">
+        <v>1.02E-47</v>
+      </c>
+      <c r="C19">
+        <v>14.464216070000001</v>
+      </c>
+      <c r="F19">
+        <v>14.7</v>
+      </c>
+      <c r="G19" s="1">
+        <v>2.1399999999999999E-29</v>
+      </c>
+      <c r="H19">
+        <v>11.191409569999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>28</v>
+      </c>
+      <c r="B20" s="1">
+        <v>2.73E-49</v>
+      </c>
+      <c r="C20">
+        <v>14.71106752</v>
+      </c>
+      <c r="F20">
+        <v>14.8</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>29</v>
+      </c>
+      <c r="B21" s="1">
+        <v>5.5999999999999999E-47</v>
+      </c>
+      <c r="C21">
+        <v>14.346153210000001</v>
+      </c>
+      <c r="F21">
+        <v>14.9</v>
+      </c>
+      <c r="G21" s="1">
+        <v>2.9399999999999999E-28</v>
+      </c>
+      <c r="H21">
+        <v>10.959338730000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>30</v>
+      </c>
+      <c r="B22" s="1">
+        <v>1.3100000000000001E-48</v>
+      </c>
+      <c r="C22">
+        <v>14.60470864</v>
+      </c>
+      <c r="F22">
+        <v>15</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F23">
+        <v>15.1</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F24">
+        <v>15.2</v>
+      </c>
+      <c r="G24" s="1">
+        <v>6.7099999999999997E-29</v>
+      </c>
+      <c r="H24">
+        <v>11.08995243</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F25">
+        <v>15.3</v>
+      </c>
+      <c r="G25" s="1">
+        <v>2.7399999999999999E-36</v>
+      </c>
+      <c r="H25">
+        <v>12.52371668</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F26">
+        <v>15.4</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F27">
+        <v>15.5</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F28">
+        <v>15.6</v>
+      </c>
+      <c r="G28" s="1">
+        <v>4.9799999999999997E-25</v>
+      </c>
+      <c r="H28">
+        <v>10.264688919999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F29">
+        <v>15.7</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F30">
+        <v>15.8</v>
+      </c>
+      <c r="G30">
+        <v>1</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F31">
+        <v>15.9</v>
+      </c>
+      <c r="G31" s="1">
+        <v>1.03E-32</v>
+      </c>
+      <c r="H31">
+        <v>11.852269789999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F32">
+        <v>16</v>
+      </c>
+      <c r="G32" s="1">
+        <v>9.1100000000000005E-37</v>
+      </c>
+      <c r="H32">
+        <v>12.61052355</v>
+      </c>
+    </row>
+    <row r="33" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F33">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="G33" s="1">
+        <v>1.1000000000000001E-25</v>
+      </c>
+      <c r="H33">
+        <v>10.40999304</v>
+      </c>
+    </row>
+    <row r="34" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F34">
+        <v>16.2</v>
+      </c>
+      <c r="G34" s="1">
+        <v>3.59E-42</v>
+      </c>
+      <c r="H34">
+        <v>13.556331999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F35">
+        <v>16.3</v>
+      </c>
+      <c r="G35" s="1">
+        <v>7.3200000000000004E-33</v>
+      </c>
+      <c r="H35">
+        <v>11.879482530000001</v>
+      </c>
+    </row>
+    <row r="36" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F36">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="G36" s="1">
+        <v>5.84E-33</v>
+      </c>
+      <c r="H36">
+        <v>11.89906201</v>
+      </c>
+    </row>
+    <row r="37" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F37">
+        <v>16.5</v>
+      </c>
+      <c r="G37" s="1">
+        <v>1.6800000000000001E-39</v>
+      </c>
+      <c r="H37">
+        <v>13.097228980000001</v>
+      </c>
+    </row>
+    <row r="38" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F38">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="G38" s="1">
+        <v>7.4700000000000001E-39</v>
+      </c>
+      <c r="H38">
+        <v>12.982961250000001</v>
+      </c>
+    </row>
+    <row r="39" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F39">
+        <v>16.7</v>
+      </c>
+      <c r="G39">
+        <v>1</v>
+      </c>
+      <c r="H39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F40">
+        <v>16.8</v>
+      </c>
+      <c r="G40" s="1">
+        <v>4.15E-36</v>
+      </c>
+      <c r="H40">
+        <v>12.49012033</v>
+      </c>
+    </row>
+    <row r="41" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F41">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="G41">
+        <v>1</v>
+      </c>
+      <c r="H41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F42">
+        <v>17</v>
+      </c>
+      <c r="G42" s="1">
+        <v>3.7100000000000001E-33</v>
+      </c>
+      <c r="H42">
+        <v>11.938932769999999</v>
+      </c>
+    </row>
+    <row r="43" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F43">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="G43" s="1">
+        <v>3.1999999999999998E-35</v>
+      </c>
+      <c r="H43">
+        <v>12.32634011</v>
+      </c>
+    </row>
+    <row r="44" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F44">
+        <v>17.2</v>
+      </c>
+      <c r="G44" s="1">
+        <v>2.02E-39</v>
+      </c>
+      <c r="H44">
+        <v>13.08362245</v>
+      </c>
+    </row>
+    <row r="45" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F45">
+        <v>17.3</v>
+      </c>
+      <c r="G45" s="1">
+        <v>1.2900000000000001E-43</v>
+      </c>
+      <c r="H45">
+        <v>13.79881484</v>
+      </c>
+    </row>
+    <row r="46" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F46">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="G46" s="1">
+        <v>1.67E-41</v>
+      </c>
+      <c r="H46">
+        <v>13.443749950000001</v>
+      </c>
+    </row>
+    <row r="47" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F47">
+        <v>17.5</v>
+      </c>
+      <c r="G47" s="1">
+        <v>8.6800000000000005E-42</v>
+      </c>
+      <c r="H47">
+        <v>13.4914346</v>
+      </c>
+    </row>
+    <row r="48" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F48">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="G48" s="1">
+        <v>1.01E-32</v>
+      </c>
+      <c r="H48">
+        <v>11.853413359999999</v>
+      </c>
+    </row>
+    <row r="49" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F49">
+        <v>17.7</v>
+      </c>
+      <c r="G49" s="1">
+        <v>2.8399999999999998E-38</v>
+      </c>
+      <c r="H49">
+        <v>12.88099411</v>
+      </c>
+    </row>
+    <row r="50" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F50">
+        <v>17.8</v>
+      </c>
+      <c r="G50" s="1">
+        <v>2.1399999999999999E-39</v>
+      </c>
+      <c r="H50">
+        <v>13.07901618</v>
+      </c>
+    </row>
+    <row r="51" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F51">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="G51" s="1">
+        <v>4.6799999999999997E-42</v>
+      </c>
+      <c r="H51">
+        <v>13.537189229999999</v>
+      </c>
+    </row>
+    <row r="52" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F52">
+        <v>18</v>
+      </c>
+      <c r="G52" s="1">
+        <v>5.7399999999999997E-46</v>
+      </c>
+      <c r="H52">
+        <v>14.184003329999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>